<commit_message>
small change in code
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawei\Documents\GitHub\DKS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D4844E-5B1C-4136-8E86-88A0EE878224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DB13FC-DE94-44C6-B7A7-D1F9FB944438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -119,6 +119,9 @@
   <si>
     <t>Arbeit insgesamt 
 Stunden (7 Wochen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installed Microsoft apps and Putty (for serial coms with Pluto). Installed python extension for Visual studio, updated both SDRs to AD9361. </t>
   </si>
 </sst>
 </file>
@@ -126,15 +129,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="9">
-    <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="d\.m\.yy;@"/>
-    <numFmt numFmtId="169" formatCode="0000\-00\ 00\ 00"/>
-    <numFmt numFmtId="170" formatCode="d/m/yy;@"/>
-    <numFmt numFmtId="171" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    <numFmt numFmtId="172" formatCode="h:mm;@"/>
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="d\.m\.yy;@"/>
+    <numFmt numFmtId="167" formatCode="0000\-00\ 00\ 00"/>
+    <numFmt numFmtId="168" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    <numFmt numFmtId="170" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -575,19 +578,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -596,10 +599,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -648,25 +651,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="5">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="5">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -678,13 +681,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1">
@@ -695,59 +698,59 @@
     </xf>
   </cellXfs>
   <cellStyles count="53">
-    <cellStyle name="20 % - Akzent1" xfId="30" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="34" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="38" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="42" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="46" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="50" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="31" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="35" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="39" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="43" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="47" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="51" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="32" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="36" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="40" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="44" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="48" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="52" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="29" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="33" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="37" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="41" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="45" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="49" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="21" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="22" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="30" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="34" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="38" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="42" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="46" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="50" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="31" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="35" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="39" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="43" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="47" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="51" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="32" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="36" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="40" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="44" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="48" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="52" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="29" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="33" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="37" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="41" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="45" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="49" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="18" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="22" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="24" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="12" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Comma [0]" xfId="13" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="14" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Currency [0]" xfId="15" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Datum" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Dezimal [0]" xfId="13" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="20" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="28" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="27" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="17" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Komma" xfId="12" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Link" xfId="10" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="27" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="17" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="20" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="23" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="19" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="26" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Prozent" xfId="16" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="18" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="26" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="21" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="16" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Stunden" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Telefon" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="28" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Uhrzeit" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="23" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Währung" xfId="14" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Währung [0]" xfId="15" builtinId="7" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="25" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="24" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="25" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1136,22 +1139,22 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="53.6328125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1162,7 +1165,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1171,7 +1174,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
@@ -1187,7 +1190,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1201,25 +1204,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3">
         <v>63</v>
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle[Arbeitsstunden])</f>
-        <v>46.5</v>
+        <v>49.5</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>46.5</v>
+        <v>49.5</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6, "")</f>
-        <v>-16.5</v>
+        <v>-13.5</v>
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -1242,7 +1245,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>45600</v>
       </c>
@@ -1260,7 +1263,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>45601</v>
       </c>
@@ -1278,7 +1281,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>45602</v>
       </c>
@@ -1296,7 +1299,7 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>45607</v>
       </c>
@@ -1314,7 +1317,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>45609</v>
       </c>
@@ -1336,7 +1339,7 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>45615</v>
       </c>
@@ -1354,7 +1357,7 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>45616</v>
       </c>
@@ -1374,7 +1377,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>45618</v>
       </c>
@@ -1396,7 +1399,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>45622</v>
       </c>
@@ -1416,7 +1419,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <v>45628</v>
       </c>
@@ -1436,7 +1439,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <v>45629</v>
       </c>
@@ -1458,7 +1461,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
         <v>45631</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <v>45674</v>
       </c>
@@ -1498,21 +1501,27 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
         <v>45677</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="8">
+        <v>0.5625</v>
+      </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
+      <c r="F21" s="8">
+        <v>0.6875</v>
+      </c>
       <c r="G21" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="13"/>
-    </row>
-    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
         <f>B21+1</f>
         <v>45678</v>
@@ -1527,7 +1536,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
         <f>B22+1</f>
         <v>45679</v>
@@ -1542,7 +1551,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
         <v>45684</v>
       </c>
@@ -1556,7 +1565,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
         <v>45685</v>
       </c>
@@ -1570,7 +1579,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14">
         <v>45686</v>
       </c>
@@ -1636,19 +1645,19 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="53.6328125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1659,7 +1668,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1668,7 +1677,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1676,7 +1685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
@@ -1684,7 +1693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1698,7 +1707,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3">
         <v>72</v>
       </c>
@@ -1716,7 +1725,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -1739,7 +1748,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>45691</v>
       </c>
@@ -1753,7 +1762,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1765,7 +1774,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1777,7 +1786,7 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1789,7 +1798,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -1801,7 +1810,7 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1813,7 +1822,7 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -1825,7 +1834,7 @@
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1837,7 +1846,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1849,7 +1858,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1861,7 +1870,7 @@
       </c>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -1873,7 +1882,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1885,7 +1894,7 @@
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -1897,7 +1906,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1909,7 +1918,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -1921,7 +1930,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -1933,7 +1942,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -1945,7 +1954,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -1957,7 +1966,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>

</xml_diff>

<commit_message>
added a few codes and solved usb port problem through command iio_info -s
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DB13FC-DE94-44C6-B7A7-D1F9FB944438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187CB059-78B5-4495-82DE-E57D8BD1DD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t xml:space="preserve">Installed Microsoft apps and Putty (for serial coms with Pluto). Installed python extension for Visual studio, updated both SDRs to AD9361. </t>
+  </si>
+  <si>
+    <t>Discussion about synchronization, tested Khaleel's code and made constellation code for the noise test.</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1142,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1210,15 +1213,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle[Arbeitsstunden])</f>
-        <v>49.5</v>
+        <v>52.5</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>49.5</v>
+        <v>52.5</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6, "")</f>
-        <v>-13.5</v>
+        <v>-10.5</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -1526,15 +1529,25 @@
         <f>B21+1</f>
         <v>45678</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
+      <c r="C22" s="8">
+        <v>0.4375</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0.57013888888888886</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0.59097222222222223</v>
+      </c>
       <c r="G22" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="13"/>
+        <v>3</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7">

</xml_diff>

<commit_message>
Finished noise test code.
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187CB059-78B5-4495-82DE-E57D8BD1DD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF4065F-A256-4F73-8101-BF627476C28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Discussion about synchronization, tested Khaleel's code and made constellation code for the noise test.</t>
+  </si>
+  <si>
+    <t>Finished noise test, worked. Discussion about Gaussian noise and further work.</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1145,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1213,15 +1216,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle[Arbeitsstunden])</f>
-        <v>52.5</v>
+        <v>56.05</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>52.5</v>
+        <v>56.05</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6, "")</f>
-        <v>-10.5</v>
+        <v>-6.9500000000000028</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -1554,15 +1557,21 @@
         <f>B22+1</f>
         <v>45679</v>
       </c>
-      <c r="C23" s="8"/>
+      <c r="C23" s="8">
+        <v>0.40972222222222221</v>
+      </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
+      <c r="F23" s="8">
+        <v>0.55763888888888891</v>
+      </c>
       <c r="G23" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="13"/>
+        <v>3.5500000000000007</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7">

</xml_diff>

<commit_message>
finished self transmitting and receiving constellation code
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF4065F-A256-4F73-8101-BF627476C28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C30FFC4-509F-49DD-B303-B4CBDA5E124A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1145,7 +1145,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1577,8 +1577,12 @@
       <c r="B24" s="7">
         <v>45684</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
+      <c r="C24" s="8">
+        <v>0.40625</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="4">

</xml_diff>

<commit_message>
SDR to SDR constellation code made, still to test
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C30FFC4-509F-49DD-B303-B4CBDA5E124A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2269BED-3FCF-436A-8AF1-7E2652363A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1145,7 +1145,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1216,15 +1216,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle[Arbeitsstunden])</f>
-        <v>56.05</v>
+        <v>59.05</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>56.05</v>
+        <v>59.05</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6, "")</f>
-        <v>-6.9500000000000028</v>
+        <v>-3.9500000000000028</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -1583,11 +1583,15 @@
       <c r="D24" s="8">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
+      <c r="E24" s="8">
+        <v>0.60902777777777772</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.66111111111111109</v>
+      </c>
       <c r="G24" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H24" s="13"/>
     </row>

</xml_diff>

<commit_message>
constellation diagrams need to be modified
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2269BED-3FCF-436A-8AF1-7E2652363A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D72AB6A-5144-40B6-9F74-FD4FBE9EEE80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Finished noise test, worked. Discussion about Gaussian noise and further work.</t>
+  </si>
+  <si>
+    <t>Reliced error in constellation diagram. Talked about downsampling and signal edge estimation. Found new literature on it.</t>
   </si>
 </sst>
 </file>
@@ -1144,7 +1147,7 @@
   </sheetPr>
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -1216,15 +1219,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle[Arbeitsstunden])</f>
-        <v>59.05</v>
+        <v>62.666666666666664</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>59.05</v>
+        <v>62.666666666666664</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6, "")</f>
-        <v>-3.9500000000000028</v>
+        <v>-0.3333333333333357</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -1599,15 +1602,21 @@
       <c r="B25" s="7">
         <v>45685</v>
       </c>
-      <c r="C25" s="8"/>
+      <c r="C25" s="8">
+        <v>0.37013888888888891</v>
+      </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="F25" s="8">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="G25" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="13"/>
+        <v>3.6166666666666671</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14">

</xml_diff>

<commit_message>
just updated workinghours file, no changes in code
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,22 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D72AB6A-5144-40B6-9F74-FD4FBE9EEE80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F348CE0B-2153-4501-98D5-528BEAEC3F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="18900" windowHeight="11055" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
-    <sheet name="Feb-Mär" sheetId="2" r:id="rId2"/>
+    <sheet name="Feb" sheetId="2" r:id="rId2"/>
+    <sheet name="März-Apr" sheetId="3" r:id="rId3"/>
+    <sheet name="Mai-Jun" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Arbeitswochenstunden" localSheetId="1">'Feb-Mär'!$B$6</definedName>
+    <definedName name="Arbeitswochenstunden" localSheetId="1">Feb!$B$6</definedName>
+    <definedName name="Arbeitswochenstunden" localSheetId="3">'Mai-Jun'!$B$6</definedName>
+    <definedName name="Arbeitswochenstunden" localSheetId="2">'März-Apr'!$B$6</definedName>
     <definedName name="Arbeitswochenstunden">'Dec-Jan'!$B$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Dec-Jan'!$7:$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Feb-Mär'!$7:$7</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">Feb!$7:$7</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Mai-Jun'!$7:$7</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'März-Apr'!$7:$7</definedName>
     <definedName name="Spaltentitel1" localSheetId="1">Arbeitszeittabelle3[[#Headers],[Datumsangaben]]</definedName>
+    <definedName name="Spaltentitel1" localSheetId="3">Arbeitszeittabelle34[[#Headers],[Datumsangaben]]</definedName>
+    <definedName name="Spaltentitel1" localSheetId="2">Arbeitszeittabelle34[[#Headers],[Datumsangaben]]</definedName>
     <definedName name="Spaltentitel1">Arbeitszeittabelle[[#Headers],[Datumsangaben]]</definedName>
-    <definedName name="Spaltentitelbereich1..E6.1" localSheetId="1">'Feb-Mär'!$B$5</definedName>
+    <definedName name="Spaltentitelbereich1..E6.1" localSheetId="1">Feb!$B$5</definedName>
+    <definedName name="Spaltentitelbereich1..E6.1" localSheetId="3">'Mai-Jun'!$B$5</definedName>
+    <definedName name="Spaltentitelbereich1..E6.1" localSheetId="2">'März-Apr'!$B$5</definedName>
     <definedName name="Spaltentitelbereich1..E6.1">'Dec-Jan'!$B$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -44,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -92,9 +102,6 @@
     <t>Vom 04.11.2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Bis zum: </t>
-  </si>
-  <si>
     <t>Task</t>
   </si>
   <si>
@@ -130,7 +137,36 @@
     <t>Finished noise test, worked. Discussion about Gaussian noise and further work.</t>
   </si>
   <si>
-    <t>Reliced error in constellation diagram. Talked about downsampling and signal edge estimation. Found new literature on it.</t>
+    <t>Raeliced error in constellation diagram. Talked about downsampling and signal edge estimation. Found new literature on it.</t>
+  </si>
+  <si>
+    <t>Arbeit insgesamt 
+Stunden (4 Wochen)</t>
+  </si>
+  <si>
+    <t>Bis zum: 29.01.25</t>
+  </si>
+  <si>
+    <t>Vom 03.02.2025</t>
+  </si>
+  <si>
+    <t>Bis zum: 28.01.2025</t>
+  </si>
+  <si>
+    <t>Vom 03.03.2025</t>
+  </si>
+  <si>
+    <t>Bis zum: 25.04.2025</t>
+  </si>
+  <si>
+    <t>Vom 28.04.2025</t>
+  </si>
+  <si>
+    <t>Bis zum: 27.06.2025</t>
+  </si>
+  <si>
+    <t>Arbeit insgesamt 
+Stunden (9 Wochen)</t>
   </si>
 </sst>
 </file>
@@ -761,7 +797,13 @@
     <cellStyle name="Uhrzeit" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Warning Text" xfId="25" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -815,10 +857,10 @@
   </dxfs>
   <tableStyles count="1" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Arbeitszeittabelle" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="5"/>
-      <tableStyleElement type="headerRow" dxfId="4"/>
-      <tableStyleElement type="firstRowStripe" dxfId="3"/>
-      <tableStyleElement type="secondRowStripe" dxfId="2"/>
+      <tableStyleElement type="wholeTable" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="6"/>
+      <tableStyleElement type="firstRowStripe" dxfId="5"/>
+      <tableStyleElement type="secondRowStripe" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -844,7 +886,7 @@
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Arbeitsstunden" dataCellStyle="Stunden">
       <calculatedColumnFormula>IFERROR(IF(COUNT(Arbeitszeittabelle[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle[[#This Row],[Einstempelzeit]],0))*24,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4D7042E7-557B-424B-AA45-14E330AC962B}" name="Task" dataDxfId="1" dataCellStyle="Uhrzeit"/>
+    <tableColumn id="7" xr3:uid="{4D7042E7-557B-424B-AA45-14E330AC962B}" name="Task" dataDxfId="3" dataCellStyle="Uhrzeit"/>
   </tableColumns>
   <tableStyleInfo name="Arbeitszeittabelle" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -867,7 +909,53 @@
     <tableColumn id="6" xr3:uid="{07172383-F2DC-4AF3-B906-B204F40AC9A1}" name="Arbeitsstunden" dataCellStyle="Stunden">
       <calculatedColumnFormula>IFERROR(IF(COUNT(Arbeitszeittabelle3[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle3[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle3[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle3[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],0))*24,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F5360DB3-8D78-4A4E-995B-95A14F8A2A5C}" name="Task" dataDxfId="0" dataCellStyle="Uhrzeit"/>
+    <tableColumn id="7" xr3:uid="{F5360DB3-8D78-4A4E-995B-95A14F8A2A5C}" name="Task" dataDxfId="2" dataCellStyle="Uhrzeit"/>
+  </tableColumns>
+  <tableStyleInfo name="Arbeitszeittabelle" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Geben Sie die täglichen Anwesenheits- und Abwesenheitszeiten einschließlich Mittagspausen (Start- und Endzeiten) ein. Die tägliche Arbeitszeit, die gesamten Arbeitsstunden, die regulären Arbeitsstunden und Überstunden werden automatisch berechnet."/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27CC0D46-9FC3-4AC3-9C45-26E9DE397AED}" name="Arbeitszeittabelle34" displayName="Arbeitszeittabelle34" ref="B7:H26" totalsRowShown="0">
+  <autoFilter ref="B7:H26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{5D61E1F0-99B8-4BDB-BCFD-A1ED5DC74287}" name="Datumsangaben" dataCellStyle="Datum"/>
+    <tableColumn id="2" xr3:uid="{D946B745-1701-449B-B9F1-66D73FF52DF6}" name="Einstempelzeit" dataCellStyle="Uhrzeit"/>
+    <tableColumn id="3" xr3:uid="{6502D56D-CCF6-49A2-A2BC-F35302AB2D54}" name="Beginn der Mittagspause" dataCellStyle="Uhrzeit"/>
+    <tableColumn id="4" xr3:uid="{AED5D554-7518-47ED-8DF4-4D065A0DCCEC}" name="Ende der Mittagspause" dataCellStyle="Uhrzeit"/>
+    <tableColumn id="5" xr3:uid="{CF9BA0AC-9DBB-4CCD-A128-EF4428081075}" name="Ausstempelzeit" dataCellStyle="Uhrzeit"/>
+    <tableColumn id="6" xr3:uid="{5629D262-F8A8-4B94-A3DD-B19FCDF5C001}" name="Arbeitsstunden" dataCellStyle="Stunden">
+      <calculatedColumnFormula>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{5C4F58A5-4267-4341-BD29-DEF9F575D42E}" name="Task" dataDxfId="1" dataCellStyle="Uhrzeit"/>
+  </tableColumns>
+  <tableStyleInfo name="Arbeitszeittabelle" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Geben Sie die täglichen Anwesenheits- und Abwesenheitszeiten einschließlich Mittagspausen (Start- und Endzeiten) ein. Die tägliche Arbeitszeit, die gesamten Arbeitsstunden, die regulären Arbeitsstunden und Überstunden werden automatisch berechnet."/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{482B3FC3-E8D5-4146-B2D6-82AEC5B00C01}" name="Arbeitszeittabelle345" displayName="Arbeitszeittabelle345" ref="B7:H26" totalsRowShown="0">
+  <autoFilter ref="B7:H26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{B1B4DE99-A545-4878-8B4B-FD1984E8CB0B}" name="Datumsangaben" dataCellStyle="Datum"/>
+    <tableColumn id="2" xr3:uid="{1EBF056C-F863-4A43-A64F-EDBE8145B1E1}" name="Einstempelzeit" dataCellStyle="Uhrzeit"/>
+    <tableColumn id="3" xr3:uid="{4FC50386-78CB-46B7-8D8C-43ED6C8561FB}" name="Beginn der Mittagspause" dataCellStyle="Uhrzeit"/>
+    <tableColumn id="4" xr3:uid="{AEF2ADC8-BA3A-4E3E-A4B2-24326643105C}" name="Ende der Mittagspause" dataCellStyle="Uhrzeit"/>
+    <tableColumn id="5" xr3:uid="{A41C0C39-956A-4E00-B600-24F5364E37F7}" name="Ausstempelzeit" dataCellStyle="Uhrzeit"/>
+    <tableColumn id="6" xr3:uid="{BC7F2F1E-6213-4EA1-914A-CE51FC741A13}" name="Arbeitsstunden" dataCellStyle="Stunden">
+      <calculatedColumnFormula>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{AD564D9A-C5FA-4654-932B-BFAF08155396}" name="Task" dataDxfId="0" dataCellStyle="Uhrzeit"/>
   </tableColumns>
   <tableStyleInfo name="Arbeitszeittabelle" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1147,8 +1235,8 @@
   </sheetPr>
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1196,12 +1284,12 @@
         <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
@@ -1251,7 +1339,7 @@
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1383,7 +1471,7 @@
         <v>1.9999999999999996</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1425,7 +1513,7 @@
         <v>5.5833333333333348</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1445,7 +1533,7 @@
         <v>2.0000000000000009</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1487,7 +1575,7 @@
         <v>3</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1507,7 +1595,7 @@
         <v>1.5000000000000013</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1527,7 +1615,7 @@
         <v>3</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1552,7 +1640,7 @@
         <v>3</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1573,7 +1661,7 @@
         <v>3.5500000000000007</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1615,7 +1703,7 @@
         <v>3.6166666666666671</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1680,8 +1768,8 @@
   </sheetPr>
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1726,15 +1814,15 @@
     </row>
     <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
@@ -1748,19 +1836,20 @@
     </row>
     <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3">
-        <v>72</v>
+        <f>4*9</f>
+        <v>36</v>
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle3[Arbeitsstunden])</f>
-        <v>0</v>
+        <v>3.6000000000000005</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>0</v>
+        <v>3.6000000000000005</v>
       </c>
       <c r="E6" s="3">
-        <f>IFERROR(C6-B6, "")</f>
-        <v>-72</v>
+        <f>IFERROR(C6-B6+'Dec-Jan'!E6, "")</f>
+        <v>-32.733333333333334</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -1784,20 +1873,24 @@
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>45691</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="8">
+        <v>0.37152777777777779</v>
+      </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8">
+        <v>0.52152777777777781</v>
+      </c>
       <c r="G8" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle3[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle3[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle3[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle3[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>3.6000000000000005</v>
       </c>
       <c r="H8" s="13"/>
     </row>
@@ -2055,4 +2148,780 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9AFF4E-5C3A-495A-9B88-26D3AE3ADE68}">
+  <sheetPr>
+    <tabColor theme="4"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:H26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="3">
+        <f>8*19</f>
+        <v>152</v>
+      </c>
+      <c r="C6" s="3">
+        <f>SUBTOTAL(109,Arbeitszeittabelle34[Arbeitsstunden])</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <f>IFERROR(C6-B6+Feb!E6, "")</f>
+        <v>-184.73333333333335</v>
+      </c>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7">
+        <v>45691</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.37152777777777779</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="13"/>
+    </row>
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="13"/>
+    </row>
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="13"/>
+    </row>
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="13"/>
+    </row>
+  </sheetData>
+  <dataValidations count="25">
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:E1 D3:E4 F1:G6 H1:XFD1048576 A2:A1048576 B8:G1048576" xr:uid="{6B610A65-F9A6-45D1-B900-743AF24D6786}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Mit diesem Arbeitsblatt halten Sie die in einer Arbeitswoche geleisteten Arbeitsstunden nach. Geben Sie Datums- und Uhrzeitwerte in die Arbeitszeittabelle ein. Arbeitsstunden gesamt, reguläre Arbeitsstunden und Überstunden werden automatisch berechnet." sqref="A1" xr:uid="{8735D079-08ED-45F5-97D0-9E7ED7CB32B1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Der Titel des Arbeitsblatts befindet sich in dieser Zelle. Geben Sie in den Zellen unten Details zum Mitarbeiter und zum Vorgesetzten ein." sqref="B1" xr:uid="{D7350DB0-AED6-44E6-8F3E-FC733058C63D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in der Zelle rechts den Namen, die E-Mail-Adresse und die Telefonnummer des Mitarbeiters ein." sqref="B2" xr:uid="{5346A716-5363-4085-98BD-CB017B09C2FE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Zelle den Namen des Mitarbeiters ein." sqref="C2" xr:uid="{2006C7A8-F6BC-4150-B930-390CE8B20577}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Zelle die E-Mail-Adresse des Mitarbeiters ein." sqref="D2" xr:uid="{DCAE42AE-FB36-4541-81C9-57FDAB4E94DB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Zelle die Telefonnummer des Mitarbeiters ein." sqref="E2" xr:uid="{FAA01AEA-4AC5-47CB-A1C9-02BD9627A6A0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den Namen des Vorgesetzten in der Zelle rechts ein." sqref="B3" xr:uid="{43FA2ED7-6C7C-48E4-A935-5B6C52D0250A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Zelle den Namen des Vorgesetzten ein." sqref="C3" xr:uid="{3ADF0663-8D42-4FD2-8CA6-BD7F5BBDB970}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den Anfang des Zeitraums in dieser Zelle ein." sqref="B4" xr:uid="{948357C3-0D3D-4AB4-B0FF-E58C3C573592}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie das Ende des Zeitraums in dieser Zelle ein." sqref="C4" xr:uid="{0C5FF084-B08C-41FB-8C79-D0764F301C73}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in der Zelle unten die Gesamtzahl der Arbeitswochenstunden ein." sqref="B5" xr:uid="{1D385325-7FC4-4F7A-A9FA-E206C0B87B49}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die Summe der geleisteten Arbeitsstunden wird in der Zelle unten automatisch berechnet." sqref="C5" xr:uid="{10836041-F186-4292-82E8-433DF5DC1EE0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die Summe der regulären Arbeitsstunden wird in der Zelle unten automatisch berechnet." sqref="D5" xr:uid="{83C5B048-AFC2-47B3-937A-6840C0A95CD4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Überstunden werden in der Zelle unten automatisch berechnet." sqref="E5" xr:uid="{6A9074D3-7160-4C9E-838E-C31B92336FBB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Zelle die Gesamtzahl der Arbeitswochenstunden ein." sqref="B6" xr:uid="{E28224C3-7110-4B99-9B97-03DB48AB432A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die Summe der geleisteten Arbeitsstunden wird in dieser Zelle automatisch berechnet." sqref="C6" xr:uid="{E8169C1F-B3B2-4A50-B6BC-929F04DA5EF8}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die Summe der regulären Arbeitsstunden wird in dieser Zelle automatisch berechnet." sqref="D6" xr:uid="{2232AB4F-0139-4A20-A7C7-1144EB88F029}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die Überstunden werden in dieser Zelle automatisch berechnet." sqref="E6" xr:uid="{5215B101-FFE4-4639-95F4-C3758BC6F6D9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Spalte unter dieser Überschrift das Datum ein. Verwenden Sie Überschriftsfilter, um bestimmte Einträge zu finden." sqref="B7" xr:uid="{FBFDD03D-6066-4C03-9F30-5D6CBCB12BC8}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Spalte unter dieser Überschrift die Einstempelzeit ein." sqref="C7" xr:uid="{357E5F8D-B01A-458F-91AD-5CC3D7EC0BF7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Spalte unter dieser Überschrift den Beginn der Mittagspause ein." sqref="D7" xr:uid="{110A0A84-48FB-414F-B43E-5B25102DF2D6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Spalte unter dieser Überschrift das Ende der Mittagspause ein." sqref="E7" xr:uid="{1A7BFC59-C357-4A23-8019-6981D8B5C129}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Spalte unter dieser Überschrift die Ausstempelzeitzeit ein." sqref="F7" xr:uid="{D32C8F53-5A81-4617-A3D7-9090CDE0BCA6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die geleisteten Arbeitsstunden werden in dieser Spalte unter dieser Überschrift automatisch berechnet." sqref="G7" xr:uid="{8425DFB0-B412-489C-9D89-025158C09426}"/>
+  </dataValidations>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.4" right="0.4" top="0.4" bottom="0.4" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="81" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter differentFirst="1">
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582A1930-7DDC-4A2A-ADD8-CA8EC9D44878}">
+  <sheetPr>
+    <tabColor theme="4"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:H26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="3">
+        <f>9*19</f>
+        <v>171</v>
+      </c>
+      <c r="C6" s="3">
+        <f>SUBTOTAL(109,Arbeitszeittabelle345[Arbeitsstunden])</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
+        <v>-355.73333333333335</v>
+      </c>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7">
+        <v>45691</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.37152777777777779</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="13"/>
+    </row>
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="13"/>
+    </row>
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="13"/>
+    </row>
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="4">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="13"/>
+    </row>
+  </sheetData>
+  <dataValidations count="25">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die geleisteten Arbeitsstunden werden in dieser Spalte unter dieser Überschrift automatisch berechnet." sqref="G7" xr:uid="{B9B8D752-413D-45DD-A598-4DBCAD0F16DE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Spalte unter dieser Überschrift die Ausstempelzeitzeit ein." sqref="F7" xr:uid="{21E20B4B-E322-4E98-8A67-2F62D88CA845}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Spalte unter dieser Überschrift das Ende der Mittagspause ein." sqref="E7" xr:uid="{A76B6CA2-1D1D-4ADA-A161-09BFF7B242AE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Spalte unter dieser Überschrift den Beginn der Mittagspause ein." sqref="D7" xr:uid="{3FB914C9-38BB-4704-AFEA-0E4F76E765A6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Spalte unter dieser Überschrift die Einstempelzeit ein." sqref="C7" xr:uid="{29B7E595-C550-4D43-B4DE-B7934BD973FB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Spalte unter dieser Überschrift das Datum ein. Verwenden Sie Überschriftsfilter, um bestimmte Einträge zu finden." sqref="B7" xr:uid="{38E04F3B-4CEF-4F74-9FDC-48B157359426}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die Überstunden werden in dieser Zelle automatisch berechnet." sqref="E6" xr:uid="{55206A72-ED2C-4A79-A549-C4B286D23FD1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die Summe der regulären Arbeitsstunden wird in dieser Zelle automatisch berechnet." sqref="D6" xr:uid="{2A5A1220-47A5-4467-9BDA-B42C14E8012F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die Summe der geleisteten Arbeitsstunden wird in dieser Zelle automatisch berechnet." sqref="C6" xr:uid="{0B80A509-193B-4E7D-9A2A-AD218F4B144D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Zelle die Gesamtzahl der Arbeitswochenstunden ein." sqref="B6" xr:uid="{52CA6FDB-AAF1-4239-8920-1EA1BEF277B0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Überstunden werden in der Zelle unten automatisch berechnet." sqref="E5" xr:uid="{F4B04329-BA9D-4D8B-83B2-2511D01CBD99}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die Summe der regulären Arbeitsstunden wird in der Zelle unten automatisch berechnet." sqref="D5" xr:uid="{25CD521E-7CFC-4994-99B4-DA2D81362D22}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die Summe der geleisteten Arbeitsstunden wird in der Zelle unten automatisch berechnet." sqref="C5" xr:uid="{312DB9E6-7386-43B2-934B-F614C7E43549}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in der Zelle unten die Gesamtzahl der Arbeitswochenstunden ein." sqref="B5" xr:uid="{7C0DEFB4-D548-4DEE-B09A-2AFF6E15FDCA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie das Ende des Zeitraums in dieser Zelle ein." sqref="C4" xr:uid="{0FBE502A-8FEA-47F6-88ED-82A74DAA90A2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den Anfang des Zeitraums in dieser Zelle ein." sqref="B4" xr:uid="{E5094096-28EE-4A1E-B751-8EFDFF8C14FF}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Zelle den Namen des Vorgesetzten ein." sqref="C3" xr:uid="{56FE92F9-125D-4D6D-9D14-6E3F41AFAAED}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den Namen des Vorgesetzten in der Zelle rechts ein." sqref="B3" xr:uid="{601DCA56-8337-4CBC-9600-0859C287B0A7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Zelle die Telefonnummer des Mitarbeiters ein." sqref="E2" xr:uid="{0A068FD0-B8C1-42B3-907D-3952A60059B4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Zelle die E-Mail-Adresse des Mitarbeiters ein." sqref="D2" xr:uid="{B2882C4F-D1C6-40F2-A871-AABD5C6A2424}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in dieser Zelle den Namen des Mitarbeiters ein." sqref="C2" xr:uid="{15DB0A2E-18B9-4692-A432-8ACA3FB4485D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in der Zelle rechts den Namen, die E-Mail-Adresse und die Telefonnummer des Mitarbeiters ein." sqref="B2" xr:uid="{D9F871D8-203A-4F04-B40F-5F22B706D8BC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Der Titel des Arbeitsblatts befindet sich in dieser Zelle. Geben Sie in den Zellen unten Details zum Mitarbeiter und zum Vorgesetzten ein." sqref="B1" xr:uid="{A18F4C84-97A5-4F96-AE04-1050620DBDDA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Mit diesem Arbeitsblatt halten Sie die in einer Arbeitswoche geleisteten Arbeitsstunden nach. Geben Sie Datums- und Uhrzeitwerte in die Arbeitszeittabelle ein. Arbeitsstunden gesamt, reguläre Arbeitsstunden und Überstunden werden automatisch berechnet." sqref="A1" xr:uid="{B92A36C2-8123-43B9-B833-A8EA9A1E80B1}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:E1 D3:E4 F1:G6 H1:XFD1048576 A2:A1048576 B8:G1048576" xr:uid="{DEAAE3DE-751B-44E5-BB8C-59C4EC6DFB90}"/>
+  </dataValidations>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.4" right="0.4" top="0.4" bottom="0.4" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="81" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter differentFirst="1">
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added algorithm to detect the signal cycle beginning and its peaks
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawei\Documents\GitHub\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F348CE0B-2153-4501-98D5-528BEAEC3F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A679B0B9-A8F6-4E8C-9588-D5FB1348C238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="18900" windowHeight="11055" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -174,15 +174,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="9">
-    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="d\.m\.yy;@"/>
-    <numFmt numFmtId="167" formatCode="0000\-00\ 00\ 00"/>
-    <numFmt numFmtId="168" formatCode="d/m/yy;@"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    <numFmt numFmtId="170" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="d\.m\.yy;@"/>
+    <numFmt numFmtId="169" formatCode="0000\-00\ 00\ 00"/>
+    <numFmt numFmtId="170" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="171" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    <numFmt numFmtId="172" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -623,19 +623,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -644,10 +644,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -696,25 +696,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="5">
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="5">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -726,13 +726,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1">
@@ -743,59 +743,59 @@
     </xf>
   </cellXfs>
   <cellStyles count="53">
-    <cellStyle name="20% - Accent1" xfId="30" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="34" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="38" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="42" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="46" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="50" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="31" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="35" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="39" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="43" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="47" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="51" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="32" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="36" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="40" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="44" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="48" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="52" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="29" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="33" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="37" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="41" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="45" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="49" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="18" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="22" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="24" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Comma" xfId="12" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Comma [0]" xfId="13" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Currency" xfId="14" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Currency [0]" xfId="15" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="30" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="34" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="38" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="42" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="46" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="50" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="31" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="35" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="39" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="43" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="47" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="51" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="32" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="36" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="40" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="44" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="48" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="52" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="29" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="33" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="37" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="41" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="45" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="49" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="21" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="22" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
     <cellStyle name="Datum" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Explanatory Text" xfId="27" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="17" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="20" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="23" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Dezimal [0]" xfId="13" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="20" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="28" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="27" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="17" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Komma" xfId="12" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Link" xfId="10" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="19" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Note" xfId="26" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="21" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="16" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="26" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Prozent" xfId="16" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="18" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Stunden" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Telefon" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="28" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Uhrzeit" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Warning Text" xfId="25" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="23" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Währung" xfId="14" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Währung [0]" xfId="15" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="25" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="24" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -1239,19 +1239,19 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1262,7 +1262,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B6" s="3">
         <v>63</v>
       </c>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7">
         <v>45600</v>
       </c>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7">
         <v>45601</v>
       </c>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7">
         <v>45602</v>
       </c>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7">
         <v>45607</v>
       </c>
@@ -1414,7 +1414,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7">
         <v>45609</v>
       </c>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="7">
         <v>45615</v>
       </c>
@@ -1454,7 +1454,7 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="7">
         <v>45616</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7">
         <v>45618</v>
       </c>
@@ -1496,7 +1496,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7">
         <v>45622</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7">
         <v>45628</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="7">
         <v>45629</v>
       </c>
@@ -1558,7 +1558,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7">
         <v>45631</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7">
         <v>45674</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="7">
         <v>45677</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="7">
         <f>B21+1</f>
         <v>45678</v>
@@ -1643,7 +1643,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="7">
         <f>B22+1</f>
         <v>45679</v>
@@ -1664,7 +1664,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="7">
         <v>45684</v>
       </c>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="7">
         <v>45685</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="14">
         <v>45686</v>
       </c>
@@ -1769,22 +1769,22 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1795,7 +1795,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B4" s="9" t="s">
         <v>29</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B6" s="3">
         <f>4*9</f>
         <v>36</v>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7">
         <v>45691</v>
       </c>
@@ -1894,10 +1894,16 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="7">
+        <v>45693</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="4">
@@ -1906,7 +1912,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1918,7 +1924,7 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1930,7 +1936,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -1942,7 +1948,7 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1954,7 +1960,7 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -1966,7 +1972,7 @@
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1978,7 +1984,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1990,7 +1996,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -2002,7 +2008,7 @@
       </c>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2014,7 +2020,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2026,7 +2032,7 @@
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2038,7 +2044,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2050,7 +2056,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2062,7 +2068,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2074,7 +2080,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -2086,7 +2092,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -2098,7 +2104,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -2162,19 +2168,19 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2185,7 +2191,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -2194,7 +2200,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -2202,7 +2208,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B4" s="9" t="s">
         <v>31</v>
       </c>
@@ -2210,7 +2216,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2224,7 +2230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B6" s="3">
         <f>8*19</f>
         <v>152</v>
@@ -2243,7 +2249,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -2266,7 +2272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7">
         <v>45691</v>
       </c>
@@ -2282,7 +2288,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -2294,7 +2300,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -2306,7 +2312,7 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -2318,7 +2324,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -2330,7 +2336,7 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -2342,7 +2348,7 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -2354,7 +2360,7 @@
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -2366,7 +2372,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -2378,7 +2384,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -2390,7 +2396,7 @@
       </c>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2402,7 +2408,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2414,7 +2420,7 @@
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2426,7 +2432,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2438,7 +2444,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2450,7 +2456,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2462,7 +2468,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -2474,7 +2480,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -2486,7 +2492,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -2550,19 +2556,19 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2573,7 +2579,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -2582,7 +2588,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -2590,7 +2596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B4" s="9" t="s">
         <v>33</v>
       </c>
@@ -2598,7 +2604,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
@@ -2612,7 +2618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B6" s="3">
         <f>9*19</f>
         <v>171</v>
@@ -2631,7 +2637,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -2654,7 +2660,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7">
         <v>45691</v>
       </c>
@@ -2670,7 +2676,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -2682,7 +2688,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -2694,7 +2700,7 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -2706,7 +2712,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -2718,7 +2724,7 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -2730,7 +2736,7 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -2742,7 +2748,7 @@
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -2754,7 +2760,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -2766,7 +2772,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -2778,7 +2784,7 @@
       </c>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2790,7 +2796,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2802,7 +2808,7 @@
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2814,7 +2820,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2826,7 +2832,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2838,7 +2844,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2850,7 +2856,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -2862,7 +2868,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -2874,7 +2880,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>

</xml_diff>

<commit_message>
advances in correlation code and matlab seq generation
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A04169-45EF-4200-A33E-E7A7BECA7CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459E84C7-70F7-4333-952A-AFA9ACE3B883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,7 +178,7 @@
     <t>Read about SDRs and Python</t>
   </si>
   <si>
-    <t xml:space="preserve">-1 hour delay </t>
+    <t>-1 hour delay Aymen</t>
   </si>
 </sst>
 </file>
@@ -1784,7 +1784,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1856,15 +1856,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle3[Arbeitsstunden])</f>
-        <v>28.6</v>
+        <v>32.683333333333337</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>28.6</v>
+        <v>32.683333333333337</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'Dec-Jan'!E6, "")</f>
-        <v>-7.7333333333333343</v>
+        <v>-3.6499999999999986</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2012,14 +2012,20 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="7">
+        <v>45707</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.69444444444444442</v>
+      </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="F14" s="8">
+        <v>0.86458333333333337</v>
+      </c>
       <c r="G14" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle3[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle3[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle3[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle3[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>4.0833333333333348</v>
       </c>
       <c r="H14" s="13"/>
     </row>
@@ -2296,7 +2302,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+Feb!E6, "")</f>
-        <v>-159.73333333333335</v>
+        <v>-155.65</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2684,7 +2690,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-330.73333333333335</v>
+        <v>-326.64999999999998</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>

<commit_message>
a lot of advance today
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459E84C7-70F7-4333-952A-AFA9ACE3B883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DACA715-8A49-44B8-85D4-62DA4E15466C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -1783,8 +1783,8 @@
   </sheetPr>
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1856,15 +1856,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle3[Arbeitsstunden])</f>
-        <v>32.683333333333337</v>
+        <v>43.35</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>32.683333333333337</v>
+        <v>36</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'Dec-Jan'!E6, "")</f>
-        <v>-3.6499999999999986</v>
+        <v>7.0166666666666657</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2030,26 +2030,38 @@
       <c r="H14" s="13"/>
     </row>
     <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
+      <c r="B15" s="7">
+        <v>45712</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.5625</v>
+      </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="8">
+        <v>0.77777777777777779</v>
+      </c>
       <c r="G15" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle3[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle3[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle3[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle3[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>5.166666666666667</v>
       </c>
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
+      <c r="B16" s="7">
+        <v>45713</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="8">
+        <v>0.8125</v>
+      </c>
       <c r="G16" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle3[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle3[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle3[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle3[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle3[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle3[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>5.4999999999999991</v>
       </c>
       <c r="H16" s="13"/>
     </row>
@@ -2221,8 +2233,8 @@
   </sheetPr>
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2294,15 +2306,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle34[Arbeitsstunden])</f>
-        <v>0</v>
+        <v>6.3333333333333348</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>0</v>
+        <v>6.3333333333333348</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+Feb!E6, "")</f>
-        <v>-155.65</v>
+        <v>-138.64999999999998</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2334,14 +2346,20 @@
         <v>45691</v>
       </c>
       <c r="C8" s="8">
-        <v>0.37152777777777779</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+        <v>0.46875</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.77430555555555558</v>
+      </c>
       <c r="G8" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>6.3333333333333348</v>
       </c>
       <c r="H8" s="13"/>
     </row>
@@ -2690,7 +2708,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-326.64999999999998</v>
+        <v>-309.64999999999998</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>

<commit_message>
made threshold and error code
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DACA715-8A49-44B8-85D4-62DA4E15466C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEDF934-BF9C-4A53-8D34-3EAF552C3112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2234,7 +2234,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2306,15 +2306,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle34[Arbeitsstunden])</f>
-        <v>6.3333333333333348</v>
+        <v>11.683333333333334</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>6.3333333333333348</v>
+        <v>11.683333333333334</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+Feb!E6, "")</f>
-        <v>-138.64999999999998</v>
+        <v>-133.30000000000001</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2364,14 +2364,24 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="B9" s="7">
+        <v>45720</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.46875</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="G9" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>5.35</v>
       </c>
       <c r="H9" s="13"/>
     </row>
@@ -2708,7 +2718,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-309.64999999999998</v>
+        <v>-304.3</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>

<commit_message>
Added visualizer code, not finished
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEDF934-BF9C-4A53-8D34-3EAF552C3112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2A3F1C-E2D2-40A0-AA87-F7CBFA4C2D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="18900" windowHeight="11055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -2233,8 +2233,8 @@
   </sheetPr>
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2306,15 +2306,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle34[Arbeitsstunden])</f>
-        <v>11.683333333333334</v>
+        <v>12.683333333333334</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>11.683333333333334</v>
+        <v>12.683333333333334</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+Feb!E6, "")</f>
-        <v>-133.30000000000001</v>
+        <v>-132.30000000000001</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2386,22 +2386,36 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="7">
+        <v>45721</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.44791666666666669</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8">
+        <v>0.48958333333333331</v>
+      </c>
       <c r="G10" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>0.99999999999999911</v>
       </c>
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="B11" s="7">
+        <v>45722</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.5625</v>
+      </c>
       <c r="F11" s="8"/>
       <c r="G11" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
@@ -2718,7 +2732,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-304.3</v>
+        <v>-303.3</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>

<commit_message>
two RIS code ready for demo
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFFCABA-37DB-46C6-ACA3-9A1E9675F651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0833050E-D1A1-4F01-A603-AB65F414904E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="18900" windowHeight="11055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="18900" windowHeight="11055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -179,6 +179,18 @@
   </si>
   <si>
     <t>-1 hour delay Aymen</t>
+  </si>
+  <si>
+    <t>Did some early hours to optimize code and get visualization ready</t>
+  </si>
+  <si>
+    <t>Worked with Aymen on visualization for RIS detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explained code to Aymen </t>
+  </si>
+  <si>
+    <t>17/3/25</t>
   </si>
 </sst>
 </file>
@@ -186,10 +198,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="9">
-    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="d\.m\.yy;@"/>
     <numFmt numFmtId="167" formatCode="0000\-00\ 00\ 00"/>
     <numFmt numFmtId="168" formatCode="d/m/yy;@"/>
@@ -656,10 +668,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2234,7 +2246,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2306,15 +2318,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle34[Arbeitsstunden])</f>
-        <v>18.100000000000001</v>
+        <v>33.549999999999997</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>18.100000000000001</v>
+        <v>33.549999999999997</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+Feb!E6, "")</f>
-        <v>-126.88333333333334</v>
+        <v>-111.43333333333334</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2401,7 +2413,9 @@
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
         <v>0.99999999999999911</v>
       </c>
-      <c r="H10" s="13"/>
+      <c r="H10" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
@@ -2423,41 +2437,73 @@
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
         <v>5.4166666666666679</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="13" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="B12" s="7">
+        <v>45723</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.31944444444444442</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.62986111111111109</v>
+      </c>
       <c r="G12" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="13"/>
+        <v>5.7833333333333341</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="7">
+        <v>45727</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.44791666666666669</v>
+      </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="E13" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="G13" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>3.7499999999999987</v>
       </c>
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="B14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.57638888888888884</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.76041666666666663</v>
+      </c>
       <c r="G14" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>5.9166666666666625</v>
       </c>
       <c r="H14" s="13"/>
     </row>
@@ -2734,7 +2780,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-297.88333333333333</v>
+        <v>-282.43333333333334</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>

<commit_message>
adding a lot of stuff, specially related to sync between sdrs
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9448D4-886B-4CD8-9DDB-9CDD12028A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27BB4E0-44ED-4F62-97B0-4007C24B2A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="18900" windowHeight="11055" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="18900" windowHeight="11055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="48">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>19/3/25</t>
+  </si>
+  <si>
+    <t>20/3/25</t>
+  </si>
+  <si>
+    <t>Trying to do sync between sdrs</t>
   </si>
 </sst>
 </file>
@@ -1801,8 +1807,8 @@
   </sheetPr>
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2251,8 +2257,8 @@
   </sheetPr>
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2324,15 +2330,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle34[Arbeitsstunden])</f>
-        <v>37.883333333333333</v>
+        <v>49.55</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>37.883333333333333</v>
+        <v>49.55</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+Feb!E6, "")</f>
-        <v>-107.10000000000001</v>
+        <v>-95.433333333333337</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2544,26 +2550,44 @@
       <c r="C16" s="8">
         <v>0.36805555555555558</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="D16" s="8">
+        <v>0.46527777777777779</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="G16" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>5.0833333333333313</v>
       </c>
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="B17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.76041666666666663</v>
+      </c>
       <c r="G17" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="13"/>
+        <v>6.5833333333333321</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
@@ -2802,7 +2826,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-278.10000000000002</v>
+        <v>-266.43333333333334</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>

<commit_message>
A lot of work on sync python codes
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27BB4E0-44ED-4F62-97B0-4007C24B2A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56D41C7-9C49-4FA3-9431-8F7F34FC0405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="18900" windowHeight="11055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>Trying to do sync between sdrs</t>
+  </si>
+  <si>
+    <t>24/3/25</t>
   </si>
 </sst>
 </file>
@@ -2258,7 +2261,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2330,15 +2333,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle34[Arbeitsstunden])</f>
-        <v>49.55</v>
+        <v>54.3</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>49.55</v>
+        <v>54.3</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+Feb!E6, "")</f>
-        <v>-95.433333333333337</v>
+        <v>-90.683333333333337</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2590,14 +2593,20 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
+      <c r="B18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="8">
+        <v>0.57291666666666663</v>
+      </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="F18" s="8">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="G18" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>4.7500000000000018</v>
       </c>
       <c r="H18" s="13"/>
     </row>
@@ -2826,7 +2835,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-266.43333333333334</v>
+        <v>-261.68333333333334</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>

<commit_message>
all sync examples run. Now starting with Pluto
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56D41C7-9C49-4FA3-9431-8F7F34FC0405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7692C881-1E4E-4EAC-9161-B909602F2F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>24/3/25</t>
+  </si>
+  <si>
+    <t>26/3/25</t>
   </si>
 </sst>
 </file>
@@ -2261,7 +2264,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2333,15 +2336,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle34[Arbeitsstunden])</f>
-        <v>54.3</v>
+        <v>58.216666666666661</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>54.3</v>
+        <v>58.216666666666661</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+Feb!E6, "")</f>
-        <v>-90.683333333333337</v>
+        <v>-86.766666666666666</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2611,14 +2614,20 @@
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
+      <c r="B19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0.59375</v>
+      </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="F19" s="8">
+        <v>0.75694444444444442</v>
+      </c>
       <c r="G19" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>3.9166666666666661</v>
       </c>
       <c r="H19" s="13"/>
     </row>
@@ -2835,7 +2844,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-261.68333333333334</v>
+        <v>-257.76666666666665</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>

<commit_message>
added function to read freq offset envelope
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E221C84-6C19-4D0F-889F-553FD3F816FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EBF317-7B0C-45B7-BDC9-92D341656C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="18900" windowHeight="11055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -2273,7 +2273,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2714,7 +2714,7 @@
     </row>
     <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
-        <v>45752</v>
+        <v>45754</v>
       </c>
       <c r="C24" s="8">
         <v>0.36458333333333331</v>
@@ -2736,10 +2736,14 @@
     </row>
     <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
-        <v>45754</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
+        <v>45756</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0.5</v>
+      </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="4">

</xml_diff>

<commit_message>
finished function but need to adjust amount of array blocks
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EBF317-7B0C-45B7-BDC9-92D341656C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80628680-7892-4726-96AD-AD4515767328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="18900" windowHeight="11055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -2273,7 +2273,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2345,15 +2345,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle34[Arbeitsstunden])</f>
-        <v>80.466666666666654</v>
+        <v>84.966666666666654</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>80.466666666666654</v>
+        <v>84.966666666666654</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+Feb!E6, "")</f>
-        <v>-64.51666666666668</v>
+        <v>-60.01666666666668</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2744,18 +2744,28 @@
       <c r="D25" s="8">
         <v>0.5</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="E25" s="8">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.6875</v>
+      </c>
       <c r="G25" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>4.4999999999999982</v>
       </c>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
+      <c r="B26" s="7">
+        <v>45757</v>
+      </c>
+      <c r="C26" s="15">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="D26" s="15">
+        <v>0.4201388888888889</v>
+      </c>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="16">
@@ -2893,7 +2903,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-235.51666666666668</v>
+        <v>-231.01666666666668</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>

<commit_message>
added code to see signal components
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408CCE52-7B0A-4AA9-9655-6D6479327E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1379D9BB-80AB-4D6C-B491-E439A5E1CD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>14/4/25</t>
+  </si>
+  <si>
+    <t>16/4/25</t>
   </si>
 </sst>
 </file>
@@ -978,8 +981,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27CC0D46-9FC3-4AC3-9C45-26E9DE397AED}" name="Arbeitszeittabelle34" displayName="Arbeitszeittabelle34" ref="B7:H28" totalsRowShown="0">
-  <autoFilter ref="B7:H28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27CC0D46-9FC3-4AC3-9C45-26E9DE397AED}" name="Arbeitszeittabelle34" displayName="Arbeitszeittabelle34" ref="B7:H29" totalsRowShown="0">
+  <autoFilter ref="B7:H29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{5D61E1F0-99B8-4BDB-BCFD-A1ED5DC74287}" name="Datumsangaben" dataCellStyle="Datum"/>
     <tableColumn id="2" xr3:uid="{D946B745-1701-449B-B9F1-66D73FF52DF6}" name="Einstempelzeit" dataCellStyle="Uhrzeit"/>
@@ -2273,10 +2276,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H28"/>
+  <dimension ref="B1:H29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2348,15 +2351,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle34[Arbeitsstunden])</f>
-        <v>88.55</v>
+        <v>92.666666666666657</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>88.55</v>
+        <v>92.666666666666657</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+Feb!E6, "")</f>
-        <v>-56.433333333333337</v>
+        <v>-52.316666666666677</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2802,16 +2805,34 @@
       <c r="C28" s="15">
         <v>0.3611111111111111</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15">
         <v>0.5</v>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
       <c r="G28" s="16">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="H28" s="13"/>
+    </row>
+    <row r="29" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="15">
+        <v>0.47430555555555554</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="G29" s="16">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0.78333333333333321</v>
+      </c>
+      <c r="H29" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="25">
@@ -2942,7 +2963,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-227.43333333333334</v>
+        <v>-223.31666666666666</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>

<commit_message>
sync finally done, moving on to integrate RIS. Added final phase corr plot
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1379D9BB-80AB-4D6C-B491-E439A5E1CD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68334A5-A19E-46DD-963E-B9105261128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>16/4/25</t>
+  </si>
+  <si>
+    <t>17/4/25</t>
   </si>
 </sst>
 </file>
@@ -981,8 +984,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27CC0D46-9FC3-4AC3-9C45-26E9DE397AED}" name="Arbeitszeittabelle34" displayName="Arbeitszeittabelle34" ref="B7:H29" totalsRowShown="0">
-  <autoFilter ref="B7:H29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27CC0D46-9FC3-4AC3-9C45-26E9DE397AED}" name="Arbeitszeittabelle34" displayName="Arbeitszeittabelle34" ref="B7:H30" totalsRowShown="0">
+  <autoFilter ref="B7:H30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{5D61E1F0-99B8-4BDB-BCFD-A1ED5DC74287}" name="Datumsangaben" dataCellStyle="Datum"/>
     <tableColumn id="2" xr3:uid="{D946B745-1701-449B-B9F1-66D73FF52DF6}" name="Einstempelzeit" dataCellStyle="Uhrzeit"/>
@@ -2276,9 +2279,9 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H29"/>
+  <dimension ref="B1:H30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -2351,15 +2354,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle34[Arbeitsstunden])</f>
-        <v>92.666666666666657</v>
+        <v>98.416666666666657</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>92.666666666666657</v>
+        <v>98.416666666666657</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+Feb!E6, "")</f>
-        <v>-52.316666666666677</v>
+        <v>-46.566666666666677</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2823,16 +2826,38 @@
       <c r="C29" s="15">
         <v>0.47430555555555554</v>
       </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
+      <c r="D29" s="15">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="E29" s="15">
+        <v>0.63541666666666663</v>
+      </c>
       <c r="F29" s="15">
-        <v>0.50694444444444442</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="G29" s="16">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0.78333333333333321</v>
+        <v>4.5333333333333332</v>
       </c>
       <c r="H29" s="13"/>
+    </row>
+    <row r="30" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="15">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G30" s="16">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>1.9999999999999982</v>
+      </c>
+      <c r="H30" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="25">
@@ -2963,7 +2988,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-223.31666666666666</v>
+        <v>-217.56666666666666</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>

<commit_message>
modified fine freq off corr function to save previous correction. Works nice as the value stabilices around 15Hz
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68334A5-A19E-46DD-963E-B9105261128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3389514A-575B-49CD-8DD7-B15599AD6F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>17/4/25</t>
+  </si>
+  <si>
+    <t>18/4/25</t>
+  </si>
+  <si>
+    <t>22/4/25</t>
   </si>
 </sst>
 </file>
@@ -984,8 +990,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27CC0D46-9FC3-4AC3-9C45-26E9DE397AED}" name="Arbeitszeittabelle34" displayName="Arbeitszeittabelle34" ref="B7:H30" totalsRowShown="0">
-  <autoFilter ref="B7:H30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27CC0D46-9FC3-4AC3-9C45-26E9DE397AED}" name="Arbeitszeittabelle34" displayName="Arbeitszeittabelle34" ref="B7:H32" totalsRowShown="0">
+  <autoFilter ref="B7:H32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{5D61E1F0-99B8-4BDB-BCFD-A1ED5DC74287}" name="Datumsangaben" dataCellStyle="Datum"/>
     <tableColumn id="2" xr3:uid="{D946B745-1701-449B-B9F1-66D73FF52DF6}" name="Einstempelzeit" dataCellStyle="Uhrzeit"/>
@@ -2279,10 +2285,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H30"/>
+  <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2354,15 +2360,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle34[Arbeitsstunden])</f>
-        <v>98.416666666666657</v>
+        <v>105.16666666666666</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>98.416666666666657</v>
+        <v>105.16666666666666</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+Feb!E6, "")</f>
-        <v>-46.566666666666677</v>
+        <v>-39.816666666666677</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2858,6 +2864,42 @@
         <v>1.9999999999999982</v>
       </c>
       <c r="H30" s="13"/>
+    </row>
+    <row r="31" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="15">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15">
+        <v>0.59375</v>
+      </c>
+      <c r="G31" s="16">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>3.4999999999999996</v>
+      </c>
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="15">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15">
+        <v>0.8125</v>
+      </c>
+      <c r="G32" s="16">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>3.2499999999999991</v>
+      </c>
+      <c r="H32" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="25">
@@ -2988,7 +3030,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-217.56666666666666</v>
+        <v>-210.81666666666666</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>

<commit_message>
Did probes, corrected code... still need to do more. The code has a weird part
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3389514A-575B-49CD-8DD7-B15599AD6F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{776072E1-FE81-4806-8361-F4A6A3BEBC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,6 +37,7 @@
     <definedName name="Spaltentitelbereich1..E6.1">'Dec-Jan'!$B$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="60">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -233,6 +234,12 @@
   </si>
   <si>
     <t>22/4/25</t>
+  </si>
+  <si>
+    <t>23/4/25</t>
+  </si>
+  <si>
+    <t>24/4/25</t>
   </si>
 </sst>
 </file>
@@ -924,7 +931,7 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16">
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Arbeitszeittabelle" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="7"/>
       <tableStyleElement type="headerRow" dxfId="6"/>
@@ -990,8 +997,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27CC0D46-9FC3-4AC3-9C45-26E9DE397AED}" name="Arbeitszeittabelle34" displayName="Arbeitszeittabelle34" ref="B7:H32" totalsRowShown="0">
-  <autoFilter ref="B7:H32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27CC0D46-9FC3-4AC3-9C45-26E9DE397AED}" name="Arbeitszeittabelle34" displayName="Arbeitszeittabelle34" ref="B7:H34" totalsRowShown="0">
+  <autoFilter ref="B7:H34" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{5D61E1F0-99B8-4BDB-BCFD-A1ED5DC74287}" name="Datumsangaben" dataCellStyle="Datum"/>
     <tableColumn id="2" xr3:uid="{D946B745-1701-449B-B9F1-66D73FF52DF6}" name="Einstempelzeit" dataCellStyle="Uhrzeit"/>
@@ -2285,10 +2292,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H32"/>
+  <dimension ref="B1:H34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2360,15 +2367,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle34[Arbeitsstunden])</f>
-        <v>105.16666666666666</v>
+        <v>111.91666666666666</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>105.16666666666666</v>
+        <v>111.91666666666666</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+Feb!E6, "")</f>
-        <v>-39.816666666666677</v>
+        <v>-33.066666666666677</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2900,6 +2907,42 @@
         <v>3.2499999999999991</v>
       </c>
       <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15">
+        <v>0.8125</v>
+      </c>
+      <c r="G33" s="16">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>4.5</v>
+      </c>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="15">
+        <v>0.71875</v>
+      </c>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15">
+        <v>0.8125</v>
+      </c>
+      <c r="G34" s="16">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>2.25</v>
+      </c>
+      <c r="H34" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="25">
@@ -3030,7 +3073,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-210.81666666666666</v>
+        <v>-204.06666666666666</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>

<commit_message>
saved in the middle
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{776072E1-FE81-4806-8361-F4A6A3BEBC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4367BC81-A4EC-4629-B120-A89CEB5A5335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,6 @@
     <definedName name="Spaltentitelbereich1..E6.1">'Dec-Jan'!$B$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -55,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -240,6 +239,9 @@
   </si>
   <si>
     <t>24/4/25</t>
+  </si>
+  <si>
+    <t>28/4/25</t>
   </si>
 </sst>
 </file>
@@ -759,7 +761,7 @@
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -816,6 +818,9 @@
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="8" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="53">
@@ -997,8 +1002,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27CC0D46-9FC3-4AC3-9C45-26E9DE397AED}" name="Arbeitszeittabelle34" displayName="Arbeitszeittabelle34" ref="B7:H34" totalsRowShown="0">
-  <autoFilter ref="B7:H34" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27CC0D46-9FC3-4AC3-9C45-26E9DE397AED}" name="Arbeitszeittabelle34" displayName="Arbeitszeittabelle34" ref="B7:H35" totalsRowShown="0">
+  <autoFilter ref="B7:H35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{5D61E1F0-99B8-4BDB-BCFD-A1ED5DC74287}" name="Datumsangaben" dataCellStyle="Datum"/>
     <tableColumn id="2" xr3:uid="{D946B745-1701-449B-B9F1-66D73FF52DF6}" name="Einstempelzeit" dataCellStyle="Uhrzeit"/>
@@ -2292,10 +2297,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H34"/>
+  <dimension ref="B1:H35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2944,9 +2949,29 @@
       </c>
       <c r="H34" s="13"/>
     </row>
+    <row r="35" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="19">
+        <v>0.46875</v>
+      </c>
+      <c r="D35" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E35" s="15">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="F35" s="15"/>
+      <c r="G35" s="16">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="13"/>
+    </row>
   </sheetData>
   <dataValidations count="25">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:E1 D3:E4 F1:G6 H1:XFD1048576 A2:A1048576 B8:G1048576" xr:uid="{6B610A65-F9A6-45D1-B900-743AF24D6786}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:E1 D3:E4 F1:G6 H1:XFD1048576 A2:A1048576 C35 B8:G34 B37:G1048576 B35:B36 D35:G36" xr:uid="{6B610A65-F9A6-45D1-B900-743AF24D6786}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Mit diesem Arbeitsblatt halten Sie die in einer Arbeitswoche geleisteten Arbeitsstunden nach. Geben Sie Datums- und Uhrzeitwerte in die Arbeitszeittabelle ein. Arbeitsstunden gesamt, reguläre Arbeitsstunden und Überstunden werden automatisch berechnet." sqref="A1" xr:uid="{8735D079-08ED-45F5-97D0-9E7ED7CB32B1}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Der Titel des Arbeitsblatts befindet sich in dieser Zelle. Geben Sie in den Zellen unten Details zum Mitarbeiter und zum Vorgesetzten ein." sqref="B1" xr:uid="{D7350DB0-AED6-44E6-8F3E-FC733058C63D}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in der Zelle rechts den Namen, die E-Mail-Adresse und die Telefonnummer des Mitarbeiters ein." sqref="B2" xr:uid="{5346A716-5363-4085-98BD-CB017B09C2FE}"/>

</xml_diff>

<commit_message>
final codes on sync task
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4367BC81-A4EC-4629-B120-A89CEB5A5335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A38D4D-6A07-454B-BF20-4768D7F4BEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>28/4/25</t>
+  </si>
+  <si>
+    <t>All comments on sync task are here https://github.com/lauravmorenoc/DKS/blob/main/Python/Synchronization/Comments.md</t>
   </si>
 </sst>
 </file>
@@ -2300,7 +2303,7 @@
   <dimension ref="B1:H35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2372,15 +2375,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle34[Arbeitsstunden])</f>
-        <v>111.91666666666666</v>
+        <v>116.16666666666666</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>111.91666666666666</v>
+        <v>116.16666666666666</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+Feb!E6, "")</f>
-        <v>-33.066666666666677</v>
+        <v>-28.816666666666677</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -2962,12 +2965,16 @@
       <c r="E35" s="15">
         <v>0.61458333333333337</v>
       </c>
-      <c r="F35" s="15"/>
+      <c r="F35" s="15">
+        <v>0.76041666666666663</v>
+      </c>
       <c r="G35" s="16">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle34[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle34[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle34[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle34[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="13"/>
+        <v>4.2499999999999982</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="25">
@@ -3098,7 +3105,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-204.06666666666666</v>
+        <v>-199.81666666666666</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>

<commit_message>
added threading for RIS and SDR
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dks\Desktop\Laura\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FFA73B-166B-4F3E-B1F1-A4C6A4B68D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AFA801-2801-4999-993E-3820E58B8A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="2595" windowWidth="18900" windowHeight="11055" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -255,10 +255,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="9">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="d\.m\.yy;@"/>
     <numFmt numFmtId="167" formatCode="0000\-00\ 00\ 00"/>
     <numFmt numFmtId="168" formatCode="d/m/yy;@"/>
@@ -725,10 +725,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3055,7 +3055,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3127,15 +3127,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle345[Arbeitsstunden])</f>
-        <v>4.3666666666666645</v>
+        <v>10.949999999999996</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>4.3666666666666645</v>
+        <v>10.949999999999996</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-192.11666666666667</v>
+        <v>-185.53333333333336</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -3193,10 +3193,12 @@
       <c r="E9" s="8">
         <v>0.61805555555555558</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="8">
+        <v>0.8125</v>
+      </c>
       <c r="G9" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>6.5833333333333321</v>
       </c>
       <c r="H9" s="13"/>
     </row>

</xml_diff>

<commit_message>
Demo codes commented and PDF guide added
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawei\Documents\GitHub\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E70314-5B95-414E-9050-51CFADB6ED32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C890AEB9-DCF2-4F5E-A304-A0910A552B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="2595" windowWidth="18900" windowHeight="11055" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -248,6 +248,15 @@
   </si>
   <si>
     <t>29/4/25</t>
+  </si>
+  <si>
+    <t>Got all equipment ready for demo</t>
+  </si>
+  <si>
+    <t>Test on equitment and codes for demo</t>
+  </si>
+  <si>
+    <t>Organized code for demo and writing demo guide</t>
   </si>
 </sst>
 </file>
@@ -830,59 +839,59 @@
     </xf>
   </cellXfs>
   <cellStyles count="53">
-    <cellStyle name="20% - Accent1" xfId="30" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="34" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="38" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="42" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="46" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="50" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="31" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="35" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="39" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="43" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="47" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="51" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="32" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="36" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="40" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="44" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="48" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="52" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="29" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="33" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="37" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="41" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="45" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="49" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="18" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="22" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="24" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Comma" xfId="12" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Comma [0]" xfId="13" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Currency" xfId="14" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Currency [0]" xfId="15" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="30" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="34" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="38" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="42" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="46" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="50" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="31" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="35" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="39" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="43" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="47" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="51" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="32" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="36" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="40" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="44" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="48" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="52" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="29" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="33" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="37" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="41" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="45" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="49" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="21" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="22" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
     <cellStyle name="Datum" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Explanatory Text" xfId="27" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="17" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="20" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="23" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Dezimal [0]" xfId="13" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="20" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="28" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="27" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="17" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Komma" xfId="12" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Link" xfId="10" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="19" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Note" xfId="26" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="21" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="16" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="26" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Prozent" xfId="16" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="18" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Stunden" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Telefon" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="28" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Uhrzeit" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Warning Text" xfId="25" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="23" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Währung" xfId="14" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Währung [0]" xfId="15" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="25" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="24" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -1326,19 +1335,19 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1349,7 +1358,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1358,7 +1367,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1366,7 +1375,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
@@ -1374,7 +1383,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1388,7 +1397,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B6" s="3">
         <v>63</v>
       </c>
@@ -1406,7 +1415,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -1429,7 +1438,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7">
         <v>45600</v>
       </c>
@@ -1447,7 +1456,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7">
         <v>45601</v>
       </c>
@@ -1465,7 +1474,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7">
         <v>45602</v>
       </c>
@@ -1483,7 +1492,7 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7">
         <v>45607</v>
       </c>
@@ -1501,7 +1510,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7">
         <v>45609</v>
       </c>
@@ -1523,7 +1532,7 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="7">
         <v>45615</v>
       </c>
@@ -1541,7 +1550,7 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="7">
         <v>45616</v>
       </c>
@@ -1561,7 +1570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7">
         <v>45618</v>
       </c>
@@ -1583,7 +1592,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7">
         <v>45622</v>
       </c>
@@ -1603,7 +1612,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7">
         <v>45628</v>
       </c>
@@ -1623,7 +1632,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="7">
         <v>45629</v>
       </c>
@@ -1645,7 +1654,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7">
         <v>45631</v>
       </c>
@@ -1665,7 +1674,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7">
         <v>45674</v>
       </c>
@@ -1685,7 +1694,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="7">
         <v>45677</v>
       </c>
@@ -1705,7 +1714,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="7">
         <f>B21+1</f>
         <v>45678</v>
@@ -1730,7 +1739,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="7">
         <f>B22+1</f>
         <v>45679</v>
@@ -1751,7 +1760,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="7">
         <v>45684</v>
       </c>
@@ -1773,7 +1782,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="7">
         <v>45685</v>
       </c>
@@ -1793,7 +1802,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="14">
         <v>45686</v>
       </c>
@@ -1859,19 +1868,19 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1882,7 +1891,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1891,7 +1900,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1899,7 +1908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B4" s="9" t="s">
         <v>29</v>
       </c>
@@ -1907,7 +1916,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1921,7 +1930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B6" s="3">
         <f>4*9</f>
         <v>36</v>
@@ -1940,7 +1949,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -1963,7 +1972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7">
         <v>45691</v>
       </c>
@@ -1983,7 +1992,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7">
         <v>45693</v>
       </c>
@@ -2007,7 +2016,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7">
         <v>45694</v>
       </c>
@@ -2027,7 +2036,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7">
         <v>45700</v>
       </c>
@@ -2045,7 +2054,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7">
         <v>45701</v>
       </c>
@@ -2063,7 +2072,7 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="7">
         <v>45706</v>
       </c>
@@ -2083,7 +2092,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="7">
         <v>45707</v>
       </c>
@@ -2101,7 +2110,7 @@
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7">
         <v>45712</v>
       </c>
@@ -2119,7 +2128,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7">
         <v>45713</v>
       </c>
@@ -2137,7 +2146,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -2149,7 +2158,7 @@
       </c>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2161,7 +2170,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2173,7 +2182,7 @@
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2185,7 +2194,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2197,7 +2206,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2209,7 +2218,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2221,7 +2230,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -2233,7 +2242,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -2245,7 +2254,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -2309,19 +2318,19 @@
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2332,7 +2341,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -2341,7 +2350,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -2349,7 +2358,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B4" s="9" t="s">
         <v>31</v>
       </c>
@@ -2357,7 +2366,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2371,7 +2380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B6" s="3">
         <f>8*19</f>
         <v>152</v>
@@ -2390,7 +2399,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -2413,7 +2422,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7">
         <v>45691</v>
       </c>
@@ -2435,7 +2444,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7">
         <v>45720</v>
       </c>
@@ -2457,7 +2466,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7">
         <v>45721</v>
       </c>
@@ -2477,7 +2486,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7">
         <v>45722</v>
       </c>
@@ -2501,7 +2510,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7">
         <v>45723</v>
       </c>
@@ -2525,7 +2534,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="7">
         <v>45727</v>
       </c>
@@ -2547,7 +2556,7 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="7" t="s">
         <v>43</v>
       </c>
@@ -2569,7 +2578,7 @@
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7" t="s">
         <v>44</v>
       </c>
@@ -2591,7 +2600,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>45</v>
       </c>
@@ -2613,7 +2622,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7" t="s">
         <v>46</v>
       </c>
@@ -2637,7 +2646,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="7" t="s">
         <v>48</v>
       </c>
@@ -2655,7 +2664,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7" t="s">
         <v>49</v>
       </c>
@@ -2673,7 +2682,7 @@
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7" t="s">
         <v>50</v>
       </c>
@@ -2691,7 +2700,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="7" t="s">
         <v>51</v>
       </c>
@@ -2709,7 +2718,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="7" t="s">
         <v>52</v>
       </c>
@@ -2727,7 +2736,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="7">
         <v>45752</v>
       </c>
@@ -2745,7 +2754,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="7">
         <v>45754</v>
       </c>
@@ -2767,7 +2776,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="7">
         <v>45756</v>
       </c>
@@ -2789,7 +2798,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="7">
         <v>45757</v>
       </c>
@@ -2807,7 +2816,7 @@
       </c>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="7">
         <v>45758</v>
       </c>
@@ -2825,7 +2834,7 @@
       </c>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="14" t="s">
         <v>53</v>
       </c>
@@ -2843,7 +2852,7 @@
       </c>
       <c r="H28" s="13"/>
     </row>
-    <row r="29" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="14" t="s">
         <v>54</v>
       </c>
@@ -2865,7 +2874,7 @@
       </c>
       <c r="H29" s="13"/>
     </row>
-    <row r="30" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="14" t="s">
         <v>55</v>
       </c>
@@ -2883,7 +2892,7 @@
       </c>
       <c r="H30" s="13"/>
     </row>
-    <row r="31" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="14" t="s">
         <v>56</v>
       </c>
@@ -2901,7 +2910,7 @@
       </c>
       <c r="H31" s="13"/>
     </row>
-    <row r="32" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="14" t="s">
         <v>57</v>
       </c>
@@ -2919,7 +2928,7 @@
       </c>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="14" t="s">
         <v>58</v>
       </c>
@@ -2937,7 +2946,7 @@
       </c>
       <c r="H33" s="13"/>
     </row>
-    <row r="34" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="14" t="s">
         <v>59</v>
       </c>
@@ -2955,7 +2964,7 @@
       </c>
       <c r="H34" s="13"/>
     </row>
-    <row r="35" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="14" t="s">
         <v>60</v>
       </c>
@@ -2979,7 +2988,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="14" t="s">
         <v>62</v>
       </c>
@@ -2997,7 +3006,7 @@
       </c>
       <c r="H36" s="13"/>
     </row>
-    <row r="37" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
@@ -3054,23 +3063,23 @@
   </sheetPr>
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3081,7 +3090,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -3090,7 +3099,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -3098,7 +3107,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B4" s="9" t="s">
         <v>33</v>
       </c>
@@ -3106,7 +3115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
@@ -3120,26 +3129,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B6" s="3">
         <f>9*19</f>
         <v>171</v>
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle345[Arbeitsstunden])</f>
-        <v>17.449999999999996</v>
+        <v>22.699999999999996</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>17.449999999999996</v>
+        <v>22.699999999999996</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-179.03333333333336</v>
+        <v>-173.78333333333336</v>
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -3162,7 +3171,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="14">
         <v>45779</v>
       </c>
@@ -3180,7 +3189,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7">
         <v>45782</v>
       </c>
@@ -3202,7 +3211,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7">
         <v>45783</v>
       </c>
@@ -3220,7 +3229,7 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7">
         <v>45784</v>
       </c>
@@ -3236,45 +3245,71 @@
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
         <v>5.0000000000000009</v>
       </c>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
+      <c r="H11" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="7">
+        <v>45786</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="F12" s="8">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="G12" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
+        <v>1.0000000000000018</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="7">
+        <v>45787</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.80902777777777779</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8">
+        <v>0.92361111111111116</v>
+      </c>
       <c r="G13" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
+        <v>2.7500000000000009</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="7">
+        <v>45788</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.5</v>
+      </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="F14" s="8">
+        <v>0.5625</v>
+      </c>
       <c r="G14" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -3286,7 +3321,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -3298,7 +3333,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -3310,7 +3345,7 @@
       </c>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -3322,7 +3357,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -3334,7 +3369,7 @@
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -3346,7 +3381,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -3358,7 +3393,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -3370,7 +3405,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -3382,7 +3417,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -3394,7 +3429,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -3406,7 +3441,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -3444,7 +3479,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie in der Zelle rechts den Namen, die E-Mail-Adresse und die Telefonnummer des Mitarbeiters ein." sqref="B2" xr:uid="{D9F871D8-203A-4F04-B40F-5F22B706D8BC}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Der Titel des Arbeitsblatts befindet sich in dieser Zelle. Geben Sie in den Zellen unten Details zum Mitarbeiter und zum Vorgesetzten ein." sqref="B1" xr:uid="{A18F4C84-97A5-4F96-AE04-1050620DBDDA}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Mit diesem Arbeitsblatt halten Sie die in einer Arbeitswoche geleisteten Arbeitsstunden nach. Geben Sie Datums- und Uhrzeitwerte in die Arbeitszeittabelle ein. Arbeitsstunden gesamt, reguläre Arbeitsstunden und Überstunden werden automatisch berechnet." sqref="A1" xr:uid="{B92A36C2-8123-43B9-B833-A8EA9A1E80B1}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:E1 D3:E4 F1:G6 H1:XFD1048576 A2:A1048576 B8:G1048576" xr:uid="{DEAAE3DE-751B-44E5-BB8C-59C4EC6DFB90}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:E1 D3:E4 F1:G6 B8:G1048576 A2:A1048576 H1:XFD1048576" xr:uid="{DEAAE3DE-751B-44E5-BB8C-59C4EC6DFB90}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.4" right="0.4" top="0.4" bottom="0.4" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added optimized beamforming RIS code
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawei\Documents\GitHub\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E57ABF-8752-4618-895A-AB4BB4923B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8B2314-24A7-4769-895B-76DFE90898CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -260,6 +260,18 @@
   </si>
   <si>
     <t>Learning to use an USRP</t>
+  </si>
+  <si>
+    <t>18/5/25</t>
+  </si>
+  <si>
+    <t>Doing VNA Measurements</t>
+  </si>
+  <si>
+    <t>19/5/25</t>
+  </si>
+  <si>
+    <t>Planing new project and creating code</t>
   </si>
 </sst>
 </file>
@@ -3067,7 +3079,7 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3139,15 +3151,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle345[Arbeitsstunden])</f>
-        <v>23.366666666666664</v>
+        <v>32.783333333333331</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>23.366666666666664</v>
+        <v>32.783333333333331</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-173.11666666666667</v>
+        <v>-163.70000000000002</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -3321,38 +3333,60 @@
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="8">
+        <v>0.80208333333333337</v>
+      </c>
       <c r="G15" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>3.4166666666666679</v>
       </c>
       <c r="H15" s="13" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
+      <c r="B16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.6875</v>
+      </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="8">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="G16" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="13"/>
+        <v>0.99999999999999911</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="B17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0.69444444444444442</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="G17" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="13"/>
+        <v>5</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="7"/>

</xml_diff>

<commit_message>
many codes for beamforming added
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawei\Documents\GitHub\DKS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8B2314-24A7-4769-895B-76DFE90898CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B8FF1E-5D1B-480F-9D00-85373BA63447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="72">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>Planing new project and creating code</t>
+  </si>
+  <si>
+    <t>20/5/25</t>
   </si>
 </sst>
 </file>
@@ -854,59 +857,59 @@
     </xf>
   </cellXfs>
   <cellStyles count="53">
-    <cellStyle name="20 % - Akzent1" xfId="30" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="34" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="38" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="42" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="46" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="50" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="31" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="35" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="39" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="43" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="47" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="51" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="32" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="36" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="40" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="44" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="48" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="52" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="29" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="33" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="37" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="41" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="45" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="49" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="21" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="22" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="30" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="34" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="38" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="42" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="46" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="50" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="31" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="35" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="39" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="43" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="47" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="51" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="32" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="36" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="40" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="44" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="48" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="52" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="29" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="33" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="37" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="41" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="45" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="49" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="18" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="22" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="24" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="12" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Comma [0]" xfId="13" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="14" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Currency [0]" xfId="15" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Datum" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Dezimal [0]" xfId="13" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="20" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="28" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="27" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="17" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Komma" xfId="12" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Link" xfId="10" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="27" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="17" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="20" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="23" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="19" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="26" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Prozent" xfId="16" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="18" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="26" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="21" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="16" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Stunden" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Telefon" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="28" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Uhrzeit" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="23" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Währung" xfId="14" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Währung [0]" xfId="15" builtinId="7" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="25" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="24" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="25" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -1350,19 +1353,19 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1373,7 +1376,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1382,7 +1385,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1390,7 +1393,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
@@ -1398,7 +1401,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1412,7 +1415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3">
         <v>63</v>
       </c>
@@ -1430,7 +1433,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>45600</v>
       </c>
@@ -1471,7 +1474,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>45601</v>
       </c>
@@ -1489,7 +1492,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>45602</v>
       </c>
@@ -1507,7 +1510,7 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>45607</v>
       </c>
@@ -1525,7 +1528,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>45609</v>
       </c>
@@ -1547,7 +1550,7 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>45615</v>
       </c>
@@ -1565,7 +1568,7 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>45616</v>
       </c>
@@ -1585,7 +1588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>45618</v>
       </c>
@@ -1607,7 +1610,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>45622</v>
       </c>
@@ -1627,7 +1630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <v>45628</v>
       </c>
@@ -1647,7 +1650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <v>45629</v>
       </c>
@@ -1669,7 +1672,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
         <v>45631</v>
       </c>
@@ -1689,7 +1692,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <v>45674</v>
       </c>
@@ -1709,7 +1712,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
         <v>45677</v>
       </c>
@@ -1729,7 +1732,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
         <f>B21+1</f>
         <v>45678</v>
@@ -1754,7 +1757,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
         <f>B22+1</f>
         <v>45679</v>
@@ -1775,7 +1778,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
         <v>45684</v>
       </c>
@@ -1797,7 +1800,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
         <v>45685</v>
       </c>
@@ -1817,7 +1820,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14">
         <v>45686</v>
       </c>
@@ -1883,19 +1886,19 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1906,7 +1909,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1915,7 +1918,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1923,7 +1926,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>29</v>
       </c>
@@ -1931,7 +1934,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1945,7 +1948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3">
         <f>4*9</f>
         <v>36</v>
@@ -1964,7 +1967,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -1987,7 +1990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>45691</v>
       </c>
@@ -2007,7 +2010,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>45693</v>
       </c>
@@ -2031,7 +2034,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>45694</v>
       </c>
@@ -2051,7 +2054,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>45700</v>
       </c>
@@ -2069,7 +2072,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>45701</v>
       </c>
@@ -2087,7 +2090,7 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>45706</v>
       </c>
@@ -2107,7 +2110,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>45707</v>
       </c>
@@ -2125,7 +2128,7 @@
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>45712</v>
       </c>
@@ -2143,7 +2146,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>45713</v>
       </c>
@@ -2161,7 +2164,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -2173,7 +2176,7 @@
       </c>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2185,7 +2188,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2197,7 +2200,7 @@
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2209,7 +2212,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2221,7 +2224,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2233,7 +2236,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2245,7 +2248,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -2257,7 +2260,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -2269,7 +2272,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -2333,19 +2336,19 @@
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2356,7 +2359,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -2365,7 +2368,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -2373,7 +2376,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>31</v>
       </c>
@@ -2381,7 +2384,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2395,7 +2398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3">
         <f>8*19</f>
         <v>152</v>
@@ -2414,7 +2417,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -2437,7 +2440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>45691</v>
       </c>
@@ -2459,7 +2462,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>45720</v>
       </c>
@@ -2481,7 +2484,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>45721</v>
       </c>
@@ -2501,7 +2504,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>45722</v>
       </c>
@@ -2525,7 +2528,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>45723</v>
       </c>
@@ -2549,7 +2552,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>45727</v>
       </c>
@@ -2571,7 +2574,7 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>43</v>
       </c>
@@ -2593,7 +2596,7 @@
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>44</v>
       </c>
@@ -2615,7 +2618,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>45</v>
       </c>
@@ -2637,7 +2640,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>46</v>
       </c>
@@ -2661,7 +2664,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>48</v>
       </c>
@@ -2679,7 +2682,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>49</v>
       </c>
@@ -2697,7 +2700,7 @@
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>50</v>
       </c>
@@ -2715,7 +2718,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>51</v>
       </c>
@@ -2733,7 +2736,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>52</v>
       </c>
@@ -2751,7 +2754,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
         <v>45752</v>
       </c>
@@ -2769,7 +2772,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
         <v>45754</v>
       </c>
@@ -2791,7 +2794,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
         <v>45756</v>
       </c>
@@ -2813,7 +2816,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7">
         <v>45757</v>
       </c>
@@ -2831,7 +2834,7 @@
       </c>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7">
         <v>45758</v>
       </c>
@@ -2849,7 +2852,7 @@
       </c>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
         <v>53</v>
       </c>
@@ -2867,7 +2870,7 @@
       </c>
       <c r="H28" s="13"/>
     </row>
-    <row r="29" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
         <v>54</v>
       </c>
@@ -2889,7 +2892,7 @@
       </c>
       <c r="H29" s="13"/>
     </row>
-    <row r="30" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
         <v>55</v>
       </c>
@@ -2907,7 +2910,7 @@
       </c>
       <c r="H30" s="13"/>
     </row>
-    <row r="31" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
         <v>56</v>
       </c>
@@ -2925,7 +2928,7 @@
       </c>
       <c r="H31" s="13"/>
     </row>
-    <row r="32" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
         <v>57</v>
       </c>
@@ -2943,7 +2946,7 @@
       </c>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
         <v>58</v>
       </c>
@@ -2961,7 +2964,7 @@
       </c>
       <c r="H33" s="13"/>
     </row>
-    <row r="34" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="14" t="s">
         <v>59</v>
       </c>
@@ -2979,7 +2982,7 @@
       </c>
       <c r="H34" s="13"/>
     </row>
-    <row r="35" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="14" t="s">
         <v>60</v>
       </c>
@@ -3003,7 +3006,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
         <v>62</v>
       </c>
@@ -3021,7 +3024,7 @@
       </c>
       <c r="H36" s="13"/>
     </row>
-    <row r="37" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
@@ -3079,22 +3082,22 @@
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3105,7 +3108,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -3114,7 +3117,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>33</v>
       </c>
@@ -3130,7 +3133,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
@@ -3144,26 +3147,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3">
         <f>9*19</f>
         <v>171</v>
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle345[Arbeitsstunden])</f>
-        <v>32.783333333333331</v>
+        <v>36.699999999999996</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>32.783333333333331</v>
+        <v>36.699999999999996</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-163.70000000000002</v>
+        <v>-159.78333333333336</v>
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -3186,7 +3189,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14">
         <v>45779</v>
       </c>
@@ -3204,7 +3207,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>45782</v>
       </c>
@@ -3226,7 +3229,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>45783</v>
       </c>
@@ -3244,7 +3247,7 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>45784</v>
       </c>
@@ -3264,7 +3267,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>45786</v>
       </c>
@@ -3284,7 +3287,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>45787</v>
       </c>
@@ -3304,7 +3307,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>45788</v>
       </c>
@@ -3324,7 +3327,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>45789</v>
       </c>
@@ -3344,7 +3347,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>67</v>
       </c>
@@ -3364,7 +3367,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>69</v>
       </c>
@@ -3388,19 +3391,25 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="8">
+        <v>0.64930555555555558</v>
+      </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="F18" s="8">
+        <v>0.8125</v>
+      </c>
       <c r="G18" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>3.9166666666666661</v>
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -3412,7 +3421,7 @@
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -3424,7 +3433,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -3436,7 +3445,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -3448,7 +3457,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -3460,7 +3469,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -3472,7 +3481,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -3484,7 +3493,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>

</xml_diff>

<commit_message>
all changes adapted to one RIS already
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C24C0A0-19EE-4533-B58D-AF7BCAF2851F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191B7A9D-7DBB-4E2E-BEDB-4EB7102E4457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="78">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>28/5/25</t>
+  </si>
+  <si>
+    <t>30/5/25</t>
   </si>
 </sst>
 </file>
@@ -3096,8 +3099,8 @@
   </sheetPr>
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3169,15 +3172,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle345[Arbeitsstunden])</f>
-        <v>55.533333333333324</v>
+        <v>59.61666666666666</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>55.533333333333324</v>
+        <v>59.61666666666666</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-140.95000000000002</v>
+        <v>-136.86666666666667</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -3519,14 +3522,20 @@
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
+      <c r="B24" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="8">
+        <v>0.64236111111111116</v>
+      </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
+      <c r="F24" s="8">
+        <v>0.8125</v>
+      </c>
       <c r="G24" s="4">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>0</v>
+        <v>4.0833333333333321</v>
       </c>
       <c r="H24" s="13"/>
     </row>

</xml_diff>

<commit_message>
created Dortmund folder and got all codes ready
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawei\Documents\GitHub\DKS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDAF064-E2E0-4738-B764-C1537120A31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2E730E-F710-4AB4-9B0C-3BE2C2A603C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2710" yWindow="1250" windowWidth="16200" windowHeight="10510" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="165" yWindow="0" windowWidth="18945" windowHeight="11610" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -308,6 +308,12 @@
   </si>
   <si>
     <t>Bis zum: 31.07.2025</t>
+  </si>
+  <si>
+    <t>Created PDF guide for demo Montreal</t>
+  </si>
+  <si>
+    <t>Prepare 2 RIS demo for Dortmund, try controlling car</t>
   </si>
 </sst>
 </file>
@@ -890,59 +896,59 @@
     </xf>
   </cellXfs>
   <cellStyles count="53">
-    <cellStyle name="20 % - Akzent1" xfId="30" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="34" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="38" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="42" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="46" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="50" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="31" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="35" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="39" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="43" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="47" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="51" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="32" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="36" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="40" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="44" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="48" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="52" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="29" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="33" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="37" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="41" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="45" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="49" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="21" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="22" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="30" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="34" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="38" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="42" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="46" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="50" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="31" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="35" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="39" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="43" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="47" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="51" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="32" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="36" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="40" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="44" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="48" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="52" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="29" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="33" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="37" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="41" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="45" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="49" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="18" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="22" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="24" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="12" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Comma [0]" xfId="13" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="14" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Currency [0]" xfId="15" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Datum" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Dezimal [0]" xfId="13" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="20" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="28" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="27" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="17" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Komma" xfId="12" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Link" xfId="10" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="27" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="17" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="20" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="23" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="19" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="26" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Prozent" xfId="16" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="18" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="26" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="21" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="16" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Stunden" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Telefon" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="28" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Uhrzeit" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="23" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Währung" xfId="14" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Währung [0]" xfId="15" builtinId="7" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="25" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="24" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="25" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -1094,8 +1100,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{482B3FC3-E8D5-4146-B2D6-82AEC5B00C01}" name="Arbeitszeittabelle345" displayName="Arbeitszeittabelle345" ref="B7:H28" totalsRowShown="0">
-  <autoFilter ref="B7:H28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{482B3FC3-E8D5-4146-B2D6-82AEC5B00C01}" name="Arbeitszeittabelle345" displayName="Arbeitszeittabelle345" ref="B7:H29" totalsRowShown="0">
+  <autoFilter ref="B7:H29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{B1B4DE99-A545-4878-8B4B-FD1984E8CB0B}" name="Datumsangaben" dataCellStyle="Datum"/>
     <tableColumn id="2" xr3:uid="{1EBF056C-F863-4A43-A64F-EDBE8145B1E1}" name="Einstempelzeit" dataCellStyle="Uhrzeit"/>
@@ -1408,23 +1414,23 @@
   </sheetPr>
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1435,7 +1441,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1444,7 +1450,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1452,7 +1458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
@@ -1460,7 +1466,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1474,7 +1480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3">
         <v>63</v>
       </c>
@@ -1492,7 +1498,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -1515,7 +1521,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>45600</v>
       </c>
@@ -1533,7 +1539,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>45601</v>
       </c>
@@ -1551,7 +1557,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>45602</v>
       </c>
@@ -1569,7 +1575,7 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>45607</v>
       </c>
@@ -1587,7 +1593,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>45609</v>
       </c>
@@ -1609,7 +1615,7 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>45615</v>
       </c>
@@ -1627,7 +1633,7 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>45616</v>
       </c>
@@ -1647,7 +1653,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>45618</v>
       </c>
@@ -1669,7 +1675,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>45622</v>
       </c>
@@ -1689,7 +1695,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <v>45628</v>
       </c>
@@ -1709,7 +1715,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <v>45629</v>
       </c>
@@ -1731,7 +1737,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
         <v>45631</v>
       </c>
@@ -1751,7 +1757,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <v>45674</v>
       </c>
@@ -1771,7 +1777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
         <v>45677</v>
       </c>
@@ -1791,7 +1797,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
         <f>B21+1</f>
         <v>45678</v>
@@ -1816,7 +1822,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
         <f>B22+1</f>
         <v>45679</v>
@@ -1837,7 +1843,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
         <v>45684</v>
       </c>
@@ -1859,7 +1865,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
         <v>45685</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14">
         <v>45686</v>
       </c>
@@ -1945,19 +1951,19 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1968,7 +1974,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1977,7 +1983,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1985,7 +1991,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>29</v>
       </c>
@@ -1993,7 +1999,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
@@ -2007,7 +2013,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3">
         <f>4*9</f>
         <v>36</v>
@@ -2026,7 +2032,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -2049,7 +2055,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>45691</v>
       </c>
@@ -2069,7 +2075,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>45693</v>
       </c>
@@ -2093,7 +2099,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>45694</v>
       </c>
@@ -2113,7 +2119,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>45700</v>
       </c>
@@ -2131,7 +2137,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>45701</v>
       </c>
@@ -2149,7 +2155,7 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>45706</v>
       </c>
@@ -2169,7 +2175,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>45707</v>
       </c>
@@ -2187,7 +2193,7 @@
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>45712</v>
       </c>
@@ -2205,7 +2211,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>45713</v>
       </c>
@@ -2223,7 +2229,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -2235,7 +2241,7 @@
       </c>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2247,7 +2253,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2259,7 +2265,7 @@
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2271,7 +2277,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2283,7 +2289,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2295,7 +2301,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2307,7 +2313,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -2319,7 +2325,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -2331,7 +2337,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -2395,19 +2401,19 @@
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2418,7 +2424,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -2427,7 +2433,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -2435,7 +2441,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>31</v>
       </c>
@@ -2443,7 +2449,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2457,7 +2463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3">
         <f>8*19</f>
         <v>152</v>
@@ -2476,7 +2482,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -2499,7 +2505,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>45691</v>
       </c>
@@ -2521,7 +2527,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>45720</v>
       </c>
@@ -2543,7 +2549,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>45721</v>
       </c>
@@ -2563,7 +2569,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>45722</v>
       </c>
@@ -2587,7 +2593,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>45723</v>
       </c>
@@ -2611,7 +2617,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>45727</v>
       </c>
@@ -2633,7 +2639,7 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>43</v>
       </c>
@@ -2655,7 +2661,7 @@
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>44</v>
       </c>
@@ -2677,7 +2683,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>45</v>
       </c>
@@ -2699,7 +2705,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>46</v>
       </c>
@@ -2723,7 +2729,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>48</v>
       </c>
@@ -2741,7 +2747,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>49</v>
       </c>
@@ -2759,7 +2765,7 @@
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>50</v>
       </c>
@@ -2777,7 +2783,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>51</v>
       </c>
@@ -2795,7 +2801,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>52</v>
       </c>
@@ -2813,7 +2819,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
         <v>45752</v>
       </c>
@@ -2831,7 +2837,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
         <v>45754</v>
       </c>
@@ -2853,7 +2859,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
         <v>45756</v>
       </c>
@@ -2875,7 +2881,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7">
         <v>45757</v>
       </c>
@@ -2893,7 +2899,7 @@
       </c>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7">
         <v>45758</v>
       </c>
@@ -2911,7 +2917,7 @@
       </c>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
         <v>53</v>
       </c>
@@ -2929,7 +2935,7 @@
       </c>
       <c r="H28" s="13"/>
     </row>
-    <row r="29" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
         <v>54</v>
       </c>
@@ -2951,7 +2957,7 @@
       </c>
       <c r="H29" s="13"/>
     </row>
-    <row r="30" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
         <v>55</v>
       </c>
@@ -2969,7 +2975,7 @@
       </c>
       <c r="H30" s="13"/>
     </row>
-    <row r="31" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
         <v>56</v>
       </c>
@@ -2987,7 +2993,7 @@
       </c>
       <c r="H31" s="13"/>
     </row>
-    <row r="32" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
         <v>57</v>
       </c>
@@ -3005,7 +3011,7 @@
       </c>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
         <v>58</v>
       </c>
@@ -3023,7 +3029,7 @@
       </c>
       <c r="H33" s="13"/>
     </row>
-    <row r="34" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="14" t="s">
         <v>59</v>
       </c>
@@ -3041,7 +3047,7 @@
       </c>
       <c r="H34" s="13"/>
     </row>
-    <row r="35" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="14" t="s">
         <v>60</v>
       </c>
@@ -3065,7 +3071,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
         <v>62</v>
       </c>
@@ -3083,7 +3089,7 @@
       </c>
       <c r="H36" s="13"/>
     </row>
-    <row r="37" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
@@ -3138,25 +3144,25 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H28"/>
+  <dimension ref="B1:H29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3167,7 +3173,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -3176,7 +3182,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -3184,7 +3190,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>33</v>
       </c>
@@ -3192,7 +3198,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
@@ -3206,7 +3212,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3">
         <f>9*19</f>
         <v>171</v>
@@ -3225,7 +3231,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -3248,7 +3254,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14">
         <v>45779</v>
       </c>
@@ -3266,7 +3272,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>45782</v>
       </c>
@@ -3288,7 +3294,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>45783</v>
       </c>
@@ -3306,7 +3312,7 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>45784</v>
       </c>
@@ -3326,7 +3332,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>45786</v>
       </c>
@@ -3346,7 +3352,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>45787</v>
       </c>
@@ -3366,7 +3372,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>45788</v>
       </c>
@@ -3386,7 +3392,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>45789</v>
       </c>
@@ -3406,7 +3412,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>67</v>
       </c>
@@ -3426,7 +3432,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>69</v>
       </c>
@@ -3450,7 +3456,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>71</v>
       </c>
@@ -3468,7 +3474,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>72</v>
       </c>
@@ -3486,7 +3492,7 @@
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>73</v>
       </c>
@@ -3504,7 +3510,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>74</v>
       </c>
@@ -3522,7 +3528,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>75</v>
       </c>
@@ -3540,7 +3546,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>76</v>
       </c>
@@ -3562,7 +3568,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
         <v>77</v>
       </c>
@@ -3580,7 +3586,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
         <v>45810</v>
       </c>
@@ -3598,7 +3604,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14">
         <v>45811</v>
       </c>
@@ -3616,7 +3622,7 @@
       </c>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="14">
         <v>45812</v>
       </c>
@@ -3634,7 +3640,7 @@
       </c>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="14">
         <v>45813</v>
       </c>
@@ -3650,7 +3656,27 @@
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
         <v>2.5000000000000004</v>
       </c>
-      <c r="H28" s="13"/>
+      <c r="H28" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="14">
+        <v>45819</v>
+      </c>
+      <c r="C29" s="15">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="16">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="25">
@@ -3700,23 +3726,23 @@
   </sheetPr>
   <dimension ref="B1:H28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="53.54296875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:8" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3727,7 +3753,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -3736,7 +3762,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -3744,7 +3770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>79</v>
       </c>
@@ -3752,7 +3778,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>78</v>
       </c>
@@ -3766,7 +3792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3">
         <f>4.8*19</f>
         <v>91.2</v>
@@ -3785,7 +3811,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -3808,7 +3834,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="8"/>
@@ -3820,7 +3846,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -3832,7 +3858,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -3844,7 +3870,7 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -3856,7 +3882,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -3868,7 +3894,7 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -3880,7 +3906,7 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -3892,7 +3918,7 @@
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -3904,7 +3930,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -3916,7 +3942,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -3928,7 +3954,7 @@
       </c>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -3940,7 +3966,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -3952,7 +3978,7 @@
       </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -3964,7 +3990,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -3976,7 +4002,7 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -3988,7 +4014,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -4000,7 +4026,7 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -4012,7 +4038,7 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -4024,7 +4050,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -4036,7 +4062,7 @@
       </c>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -4048,7 +4074,7 @@
       </c>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="2:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>

</xml_diff>

<commit_message>
codes for optimization improved
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local\Desktop\DKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EB15D2-3C73-4C93-A6CA-E90916B898EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BE2C14-2262-4CDA-8EA4-C12DF0B18CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="165" yWindow="0" windowWidth="18945" windowHeight="11610" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-Jan" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="91">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -335,6 +335,9 @@
   </si>
   <si>
     <t>Back to optimized scheme</t>
+  </si>
+  <si>
+    <t>21/6/25</t>
   </si>
 </sst>
 </file>
@@ -1124,8 +1127,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{482B3FC3-E8D5-4146-B2D6-82AEC5B00C01}" name="Arbeitszeittabelle345" displayName="Arbeitszeittabelle345" ref="B7:H39" totalsRowShown="0">
-  <autoFilter ref="B7:H39" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{482B3FC3-E8D5-4146-B2D6-82AEC5B00C01}" name="Arbeitszeittabelle345" displayName="Arbeitszeittabelle345" ref="B7:H40" totalsRowShown="0">
+  <autoFilter ref="B7:H40" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{B1B4DE99-A545-4878-8B4B-FD1984E8CB0B}" name="Datumsangaben" dataCellStyle="Datum"/>
     <tableColumn id="2" xr3:uid="{1EBF056C-F863-4A43-A64F-EDBE8145B1E1}" name="Einstempelzeit" dataCellStyle="Uhrzeit"/>
@@ -3190,10 +3193,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H39"/>
+  <dimension ref="B1:H40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3265,15 +3268,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,Arbeitszeittabelle345[Arbeitsstunden])</f>
-        <v>124.94999999999999</v>
+        <v>130.78333333333333</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=Arbeitswochenstunden,C6,Arbeitswochenstunden),"")</f>
-        <v>124.94999999999999</v>
+        <v>130.78333333333333</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'März-Apr'!E6, "")</f>
-        <v>-63.53333333333336</v>
+        <v>-57.700000000000017</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -3916,13 +3919,31 @@
       <c r="D39" s="15"/>
       <c r="E39" s="15"/>
       <c r="F39" s="15">
-        <v>0.74652777777777779</v>
+        <v>0.75347222222222221</v>
       </c>
       <c r="G39" s="16">
         <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
-        <v>5.5833333333333348</v>
+        <v>5.7500000000000009</v>
       </c>
       <c r="H39" s="13"/>
+    </row>
+    <row r="40" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="15">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="G40" s="16">
+        <f>IFERROR(IF(COUNT(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]:[Ausstempelzeit]])=4,(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Ende der Mittagspause]]+Arbeitszeittabelle345[[#This Row],[Beginn der Mittagspause]]-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],IF(AND(LEN(Arbeitszeittabelle345[[#This Row],[Einstempelzeit]])&lt;&gt;0,LEN(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])&lt;&gt;0),(IF(Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]]&lt;Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],1,0)+Arbeitszeittabelle345[[#This Row],[Ausstempelzeit]])-Arbeitszeittabelle345[[#This Row],[Einstempelzeit]],0))*24,0)</f>
+        <v>5.6666666666666679</v>
+      </c>
+      <c r="H40" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="25">
@@ -4053,7 +4074,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-B6+'Mai-Jun'!E6, "")</f>
-        <v>-154.73333333333335</v>
+        <v>-148.90000000000003</v>
       </c>
       <c r="F6" s="17"/>
     </row>

</xml_diff>